<commit_message>
Integracion codigo de Fuzzy
</commit_message>
<xml_diff>
--- a/Calculos_Python/logs.xlsx
+++ b/Calculos_Python/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E216"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.06760563380281689</v>
+        <v>-0.07171232876712329</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01669014084507042</v>
+        <v>-0.1216</v>
       </c>
       <c r="D2" t="n">
-        <v>-76.32676056338028</v>
+        <v>69.56095890410958</v>
       </c>
       <c r="E2" t="n">
-        <v>-76.32676056338028</v>
+        <v>69.56095890410958</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.06718309859154929</v>
+        <v>-0.07212328767123287</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01753521126760563</v>
+        <v>-0.1212</v>
       </c>
       <c r="D3" t="n">
-        <v>-5.269436619718314</v>
+        <v>5.418493150684924</v>
       </c>
       <c r="E3" t="n">
-        <v>-5.269436619718314</v>
+        <v>5.418493150684924</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.06718309859154929</v>
+        <v>-0.07253424657534246</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01753521126760563</v>
+        <v>-0.1212</v>
       </c>
       <c r="D4" t="n">
-        <v>-5.71056338028169</v>
+        <v>5.447260273972609</v>
       </c>
       <c r="E4" t="n">
-        <v>-5.71056338028169</v>
+        <v>5.447260273972609</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.06760563380281689</v>
+        <v>-0.07253424657534246</v>
       </c>
       <c r="C5" t="n">
-        <v>0.01669014084507042</v>
+        <v>-0.1216</v>
       </c>
       <c r="D5" t="n">
-        <v>-6.187605633802812</v>
+        <v>5.077397260273973</v>
       </c>
       <c r="E5" t="n">
-        <v>-6.187605633802812</v>
+        <v>5.077397260273973</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0680281690140845</v>
+        <v>-0.07376712328767122</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01626760563380282</v>
+        <v>-0.1232</v>
       </c>
       <c r="D6" t="n">
-        <v>-6.223521126760558</v>
+        <v>6.273287671232868</v>
       </c>
       <c r="E6" t="n">
-        <v>-6.223521126760558</v>
+        <v>6.273287671232868</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.06845070422535211</v>
+        <v>-0.07417808219178082</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01584507042253521</v>
+        <v>-0.1252</v>
       </c>
       <c r="D7" t="n">
-        <v>-6.259436619718321</v>
+        <v>5.562328767123294</v>
       </c>
       <c r="E7" t="n">
-        <v>-6.259436619718321</v>
+        <v>5.562328767123294</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.06760563380281689</v>
+        <v>-0.075</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01542253521126761</v>
+        <v>-0.1248</v>
       </c>
       <c r="D8" t="n">
-        <v>-4.864225352112668</v>
+        <v>5.98972602739726</v>
       </c>
       <c r="E8" t="n">
-        <v>-4.864225352112668</v>
+        <v>5.98972602739726</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.06633802816901407</v>
+        <v>-0.07335616438356164</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01415492957746479</v>
+        <v>-0.1236</v>
       </c>
       <c r="D9" t="n">
-        <v>-4.315352112676052</v>
+        <v>3.655479452054796</v>
       </c>
       <c r="E9" t="n">
-        <v>-4.315352112676052</v>
+        <v>3.655479452054796</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.06464788732394365</v>
+        <v>-0.07006849315068493</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01246478873239436</v>
+        <v>-0.1216</v>
       </c>
       <c r="D10" t="n">
-        <v>-3.730563380281689</v>
+        <v>1.945890410958906</v>
       </c>
       <c r="E10" t="n">
-        <v>-3.730563380281689</v>
+        <v>1.945890410958906</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.06126760563380281</v>
+        <v>-0.06595890410958903</v>
       </c>
       <c r="C11" t="n">
-        <v>0.01204225352112676</v>
+        <v>-0.1188</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.678732394366203</v>
+        <v>0.9184931506849208</v>
       </c>
       <c r="E11" t="n">
-        <v>-1.678732394366203</v>
+        <v>0.9184931506849208</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.05788732394366197</v>
+        <v>-0.06308219178082192</v>
       </c>
       <c r="C12" t="n">
-        <v>0.01035211267605634</v>
+        <v>-0.1132</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.391408450704224</v>
+        <v>1.826712328767132</v>
       </c>
       <c r="E12" t="n">
-        <v>-1.391408450704224</v>
+        <v>1.826712328767132</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.05366197183098591</v>
+        <v>-0.05732876712328767</v>
       </c>
       <c r="C13" t="n">
-        <v>0.008661971830985915</v>
+        <v>-0.1072</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.1500000000000066</v>
+        <v>-1.165068493150687</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1500000000000066</v>
+        <v>-1.165068493150687</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.04859154929577465</v>
+        <v>-0.05116438356164383</v>
       </c>
       <c r="C14" t="n">
-        <v>0.007394366197183098</v>
+        <v>-0.09879999999999999</v>
       </c>
       <c r="D14" t="n">
-        <v>1.163239436619719</v>
+        <v>-1.966438356164386</v>
       </c>
       <c r="E14" t="n">
-        <v>1.163239436619719</v>
+        <v>-1.966438356164386</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.04436619718309859</v>
+        <v>-0.04746575342465753</v>
       </c>
       <c r="C15" t="n">
-        <v>0.006549295774647887</v>
+        <v>-0.09079999999999999</v>
       </c>
       <c r="D15" t="n">
-        <v>0.640140845070424</v>
+        <v>-0.006164383561642062</v>
       </c>
       <c r="E15" t="n">
-        <v>0.640140845070424</v>
+        <v>-0.006164383561642062</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.04056338028169014</v>
+        <v>-0.04294520547945205</v>
       </c>
       <c r="C16" t="n">
-        <v>0.004859154929577465</v>
+        <v>-0.08399999999999999</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5222535211267578</v>
+        <v>-1.062328767123284</v>
       </c>
       <c r="E16" t="n">
-        <v>0.5222535211267578</v>
+        <v>-1.062328767123284</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.03676056338028168</v>
+        <v>-0.03636986301369863</v>
       </c>
       <c r="C17" t="n">
-        <v>0.004014084507042253</v>
+        <v>-0.07559999999999999</v>
       </c>
       <c r="D17" t="n">
-        <v>0.845492957746484</v>
+        <v>-3.371917808219181</v>
       </c>
       <c r="E17" t="n">
-        <v>0.845492957746484</v>
+        <v>-3.371917808219181</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.03380281690140845</v>
+        <v>-0.03184931506849315</v>
       </c>
       <c r="C18" t="n">
-        <v>0.001901408450704225</v>
+        <v>-0.0664</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2146478873239408</v>
+        <v>-1.839041095890407</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2146478873239408</v>
+        <v>-1.839041095890407</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.03126760563380281</v>
+        <v>-0.02773972602739726</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0002112676056338028</v>
+        <v>-0.05839999999999999</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.01098591549295724</v>
+        <v>-1.756849315068497</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.01098591549295724</v>
+        <v>-1.756849315068497</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.02873239436619718</v>
+        <v>-0.02445205479452055</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.0006338028169014084</v>
+        <v>-0.0484</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2045070422535185</v>
+        <v>-1.247260273972601</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2045070422535185</v>
+        <v>-1.247260273972601</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.02661971830985915</v>
+        <v>-0.01952054794520548</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.00147887323943662</v>
+        <v>-0.03999999999999999</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.05704225352112591</v>
+        <v>-3.071917808219178</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.05704225352112591</v>
+        <v>-3.071917808219178</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.02619718309859155</v>
+        <v>-0.01541095890410959</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.003169014084507042</v>
+        <v>-0.0312</v>
       </c>
       <c r="D22" t="n">
-        <v>-1.785633802816901</v>
+        <v>-2.619863013698631</v>
       </c>
       <c r="E22" t="n">
-        <v>-1.785633802816901</v>
+        <v>-2.619863013698631</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.02492957746478873</v>
+        <v>-0.01006849315068493</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.004014084507042253</v>
+        <v>-0.0236</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.7956338028169012</v>
+        <v>-4.103424657534246</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.7956338028169012</v>
+        <v>-4.103424657534246</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.02492957746478873</v>
+        <v>-0.004726027397260274</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.00528169014084507</v>
+        <v>-0.0172</v>
       </c>
       <c r="D24" t="n">
-        <v>-2.119014084507042</v>
+        <v>-4.477397260273972</v>
       </c>
       <c r="E24" t="n">
-        <v>-2.119014084507042</v>
+        <v>-4.477397260273972</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.02577464788732394</v>
+        <v>-0.0006164383561643835</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.006126760563380281</v>
+        <v>-0.009599999999999999</v>
       </c>
       <c r="D25" t="n">
-        <v>-3.073098591549296</v>
+        <v>-3.655479452054795</v>
       </c>
       <c r="E25" t="n">
-        <v>-3.073098591549296</v>
+        <v>-3.655479452054795</v>
       </c>
     </row>
     <row r="26">
@@ -868,16 +868,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.02577464788732394</v>
+        <v>0.003904109589041096</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.006549295774647887</v>
+        <v>-0.0028</v>
       </c>
       <c r="D26" t="n">
-        <v>-2.190845070422535</v>
+        <v>-4.341780821917808</v>
       </c>
       <c r="E26" t="n">
-        <v>-2.190845070422535</v>
+        <v>-4.341780821917808</v>
       </c>
     </row>
     <row r="27">
@@ -885,16 +885,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.02704225352112676</v>
+        <v>0.006780821917808219</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.006971830985915493</v>
+        <v>0.004</v>
       </c>
       <c r="D27" t="n">
-        <v>-3.621971830985916</v>
+        <v>-3.063698630136986</v>
       </c>
       <c r="E27" t="n">
-        <v>-3.621971830985916</v>
+        <v>-3.063698630136986</v>
       </c>
     </row>
     <row r="28">
@@ -902,16 +902,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.02873239436619718</v>
+        <v>0.0113013698630137</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.007394366197183098</v>
+        <v>0.0092</v>
       </c>
       <c r="D28" t="n">
-        <v>-4.206760563380282</v>
+        <v>-4.859589041095889</v>
       </c>
       <c r="E28" t="n">
-        <v>-4.206760563380282</v>
+        <v>-4.859589041095889</v>
       </c>
     </row>
     <row r="29">
@@ -919,16 +919,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.03</v>
+        <v>0.01541095890410959</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.006549295774647887</v>
+        <v>0.0132</v>
       </c>
       <c r="D29" t="n">
-        <v>-3.873380281690141</v>
+        <v>-4.777397260273974</v>
       </c>
       <c r="E29" t="n">
-        <v>-3.873380281690141</v>
+        <v>-4.777397260273974</v>
       </c>
     </row>
     <row r="30">
@@ -936,16 +936,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.03169014084507042</v>
+        <v>0.01746575342465753</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.005704225352112675</v>
+        <v>0.0184</v>
       </c>
       <c r="D30" t="n">
-        <v>-4.458169014084508</v>
+        <v>-3.071917808219177</v>
       </c>
       <c r="E30" t="n">
-        <v>-4.458169014084508</v>
+        <v>-3.071917808219177</v>
       </c>
     </row>
     <row r="31">
@@ -953,16 +953,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.03338028169014085</v>
+        <v>0.01993150684931507</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.00528169014084507</v>
+        <v>0.0216</v>
       </c>
       <c r="D31" t="n">
-        <v>-4.601830985915493</v>
+        <v>-3.614383561643837</v>
       </c>
       <c r="E31" t="n">
-        <v>-4.601830985915493</v>
+        <v>-3.614383561643837</v>
       </c>
     </row>
     <row r="32">
@@ -970,16 +970,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.03422535211267606</v>
+        <v>0.02116438356164383</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.004014084507042253</v>
+        <v>0.0236</v>
       </c>
       <c r="D32" t="n">
-        <v>-3.791408450704226</v>
+        <v>-2.591095890410958</v>
       </c>
       <c r="E32" t="n">
-        <v>-3.791408450704226</v>
+        <v>-2.591095890410958</v>
       </c>
     </row>
     <row r="33">
@@ -987,16 +987,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.03633802816901408</v>
+        <v>0.02157534246575342</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.003591549295774648</v>
+        <v>0.0244</v>
       </c>
       <c r="D33" t="n">
-        <v>-5.294366197183095</v>
+        <v>-1.880136986301369</v>
       </c>
       <c r="E33" t="n">
-        <v>-5.294366197183095</v>
+        <v>-1.880136986301369</v>
       </c>
     </row>
     <row r="34">
@@ -1004,16 +1004,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.03676056338028168</v>
+        <v>0.02198630136986301</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.001901408450704225</v>
+        <v>0.0228</v>
       </c>
       <c r="D34" t="n">
-        <v>-3.56577464788732</v>
+        <v>-1.908904109589041</v>
       </c>
       <c r="E34" t="n">
-        <v>-3.56577464788732</v>
+        <v>-1.908904109589041</v>
       </c>
     </row>
     <row r="35">
@@ -1021,16 +1021,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.0380281690140845</v>
+        <v>0.02157534246575342</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.001056338028169014</v>
+        <v>0.022</v>
       </c>
       <c r="D35" t="n">
-        <v>-4.555774647887327</v>
+        <v>-1.14041095890411</v>
       </c>
       <c r="E35" t="n">
-        <v>-4.555774647887327</v>
+        <v>-1.14041095890411</v>
       </c>
     </row>
     <row r="36">
@@ -1038,16 +1038,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.03845070422535211</v>
+        <v>0.02034246575342466</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0006338028169014084</v>
+        <v>0.02</v>
       </c>
       <c r="D36" t="n">
-        <v>-3.709436619718306</v>
+        <v>-0.3143835616438364</v>
       </c>
       <c r="E36" t="n">
-        <v>-3.709436619718306</v>
+        <v>-0.3143835616438364</v>
       </c>
     </row>
     <row r="37">
@@ -1055,16 +1055,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.03929577464788732</v>
+        <v>0.0186986301369863</v>
       </c>
       <c r="C37" t="n">
-        <v>0.00147887323943662</v>
+        <v>0.0168</v>
       </c>
       <c r="D37" t="n">
-        <v>-4.222394366197182</v>
+        <v>0.1705479452054786</v>
       </c>
       <c r="E37" t="n">
-        <v>-4.222394366197182</v>
+        <v>0.1705479452054786</v>
       </c>
     </row>
     <row r="38">
@@ -1072,16 +1072,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.03929577464788732</v>
+        <v>0.01664383561643835</v>
       </c>
       <c r="C38" t="n">
-        <v>0.002323943661971831</v>
+        <v>0.0132</v>
       </c>
       <c r="D38" t="n">
-        <v>-3.340140845070422</v>
+        <v>0.6842465753424678</v>
       </c>
       <c r="E38" t="n">
-        <v>-3.340140845070422</v>
+        <v>0.6842465753424678</v>
       </c>
     </row>
     <row r="39">
@@ -1089,16 +1089,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.04014084507042253</v>
+        <v>0.01417808219178082</v>
       </c>
       <c r="C39" t="n">
-        <v>0.003169014084507042</v>
+        <v>0.0092</v>
       </c>
       <c r="D39" t="n">
-        <v>-4.294225352112676</v>
+        <v>1.226712328767123</v>
       </c>
       <c r="E39" t="n">
-        <v>-4.294225352112676</v>
+        <v>1.226712328767123</v>
       </c>
     </row>
     <row r="40">
@@ -1106,16 +1106,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.04014084507042253</v>
+        <v>0.01089041095890411</v>
       </c>
       <c r="C40" t="n">
-        <v>0.004014084507042253</v>
+        <v>0.0052</v>
       </c>
       <c r="D40" t="n">
-        <v>-3.411971830985915</v>
+        <v>2.196575342465753</v>
       </c>
       <c r="E40" t="n">
-        <v>-3.411971830985915</v>
+        <v>2.196575342465753</v>
       </c>
     </row>
     <row r="41">
@@ -1123,16 +1123,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.04014084507042253</v>
+        <v>0.008835616438356163</v>
       </c>
       <c r="C41" t="n">
-        <v>0.004859154929577465</v>
+        <v>0.0004</v>
       </c>
       <c r="D41" t="n">
-        <v>-3.411971830985915</v>
+        <v>1.23082191780822</v>
       </c>
       <c r="E41" t="n">
-        <v>-3.411971830985915</v>
+        <v>1.23082191780822</v>
       </c>
     </row>
     <row r="42">
@@ -1140,16 +1140,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.04014084507042253</v>
+        <v>0.005136986301369863</v>
       </c>
       <c r="C42" t="n">
-        <v>0.004859154929577465</v>
+        <v>-0.0032</v>
       </c>
       <c r="D42" t="n">
-        <v>-3.411971830985915</v>
+        <v>2.96917808219178</v>
       </c>
       <c r="E42" t="n">
-        <v>-3.411971830985915</v>
+        <v>2.96917808219178</v>
       </c>
     </row>
     <row r="43">
@@ -1157,16 +1157,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.04098591549295774</v>
+        <v>0.002671232876712329</v>
       </c>
       <c r="C43" t="n">
-        <v>0.004859154929577465</v>
+        <v>-0.008</v>
       </c>
       <c r="D43" t="n">
-        <v>-4.366056338028169</v>
+        <v>2.032191780821918</v>
       </c>
       <c r="E43" t="n">
-        <v>-4.366056338028169</v>
+        <v>2.032191780821918</v>
       </c>
     </row>
     <row r="44">
@@ -1174,16 +1174,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.04098591549295774</v>
+        <v>-0.0002054794520547945</v>
       </c>
       <c r="C44" t="n">
-        <v>0.004859154929577465</v>
+        <v>-0.0128</v>
       </c>
       <c r="D44" t="n">
-        <v>-3.483802816901408</v>
+        <v>2.603424657534246</v>
       </c>
       <c r="E44" t="n">
-        <v>-3.483802816901408</v>
+        <v>2.603424657534246</v>
       </c>
     </row>
     <row r="45">
@@ -1191,16 +1191,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.04183098591549295</v>
+        <v>-0.003493150684931506</v>
       </c>
       <c r="C45" t="n">
-        <v>0.004014084507042253</v>
+        <v>-0.0164</v>
       </c>
       <c r="D45" t="n">
-        <v>-4.437887323943662</v>
+        <v>3.203424657534246</v>
       </c>
       <c r="E45" t="n">
-        <v>-4.437887323943662</v>
+        <v>3.203424657534246</v>
       </c>
     </row>
     <row r="46">
@@ -1208,16 +1208,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.04225352112676056</v>
+        <v>-0.006780821917808219</v>
       </c>
       <c r="C46" t="n">
-        <v>0.003169014084507042</v>
+        <v>-0.0188</v>
       </c>
       <c r="D46" t="n">
-        <v>-4.032676056338032</v>
+        <v>3.433561643835616</v>
       </c>
       <c r="E46" t="n">
-        <v>-4.032676056338032</v>
+        <v>3.433561643835616</v>
       </c>
     </row>
     <row r="47">
@@ -1225,16 +1225,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.04267605633802816</v>
+        <v>-0.009657534246575342</v>
       </c>
       <c r="C47" t="n">
-        <v>0.003169014084507042</v>
+        <v>-0.0216</v>
       </c>
       <c r="D47" t="n">
-        <v>-4.06859154929577</v>
+        <v>3.265068493150685</v>
       </c>
       <c r="E47" t="n">
-        <v>-4.06859154929577</v>
+        <v>3.265068493150685</v>
       </c>
     </row>
     <row r="48">
@@ -1242,16 +1242,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.04267605633802816</v>
+        <v>-0.01171232876712329</v>
       </c>
       <c r="C48" t="n">
-        <v>0.002323943661971831</v>
+        <v>-0.024</v>
       </c>
       <c r="D48" t="n">
-        <v>-3.627464788732394</v>
+        <v>2.669178082191779</v>
       </c>
       <c r="E48" t="n">
-        <v>-3.627464788732394</v>
+        <v>2.669178082191779</v>
       </c>
     </row>
     <row r="49">
@@ -1259,16 +1259,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.04352112676056338</v>
+        <v>-0.01458904109589041</v>
       </c>
       <c r="C49" t="n">
-        <v>0.001056338028169014</v>
+        <v>-0.0244</v>
       </c>
       <c r="D49" t="n">
-        <v>-4.581549295774647</v>
+        <v>3.610273972602741</v>
       </c>
       <c r="E49" t="n">
-        <v>-4.581549295774647</v>
+        <v>3.610273972602741</v>
       </c>
     </row>
     <row r="50">
@@ -1276,16 +1276,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.04352112676056338</v>
+        <v>-0.015</v>
       </c>
       <c r="C50" t="n">
-        <v>0.0006338028169014084</v>
+        <v>-0.0256</v>
       </c>
       <c r="D50" t="n">
-        <v>-3.699295774647887</v>
+        <v>1.41986301369863</v>
       </c>
       <c r="E50" t="n">
-        <v>-3.699295774647887</v>
+        <v>1.41986301369863</v>
       </c>
     </row>
     <row r="51">
@@ -1293,16 +1293,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.04352112676056338</v>
+        <v>-0.01582191780821918</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.0002112676056338028</v>
+        <v>-0.0256</v>
       </c>
       <c r="D51" t="n">
-        <v>-3.699295774647887</v>
+        <v>1.847260273972602</v>
       </c>
       <c r="E51" t="n">
-        <v>-3.699295774647887</v>
+        <v>1.847260273972602</v>
       </c>
     </row>
     <row r="52">
@@ -1310,16 +1310,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.04352112676056338</v>
+        <v>-0.01664383561643835</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.001056338028169014</v>
+        <v>-0.0248</v>
       </c>
       <c r="D52" t="n">
-        <v>-3.699295774647887</v>
+        <v>1.904794520547945</v>
       </c>
       <c r="E52" t="n">
-        <v>-3.699295774647887</v>
+        <v>1.904794520547945</v>
       </c>
     </row>
     <row r="53">
@@ -1327,16 +1327,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.04352112676056338</v>
+        <v>-0.01623287671232877</v>
       </c>
       <c r="C53" t="n">
-        <v>-0.001901408450704225</v>
+        <v>-0.0228</v>
       </c>
       <c r="D53" t="n">
-        <v>-3.699295774647887</v>
+        <v>0.7664383561643837</v>
       </c>
       <c r="E53" t="n">
-        <v>-3.699295774647887</v>
+        <v>0.7664383561643837</v>
       </c>
     </row>
     <row r="54">
@@ -1344,16 +1344,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.04352112676056338</v>
+        <v>-0.01623287671232877</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.001901408450704225</v>
+        <v>-0.0204</v>
       </c>
       <c r="D54" t="n">
-        <v>-3.699295774647887</v>
+        <v>1.136301369863014</v>
       </c>
       <c r="E54" t="n">
-        <v>-3.699295774647887</v>
+        <v>1.136301369863014</v>
       </c>
     </row>
     <row r="55">
@@ -1361,16 +1361,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.04267605633802816</v>
+        <v>-0.01541095890410959</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.001901408450704225</v>
+        <v>-0.0176</v>
       </c>
       <c r="D55" t="n">
-        <v>-2.745211267605633</v>
+        <v>0.3390410958904114</v>
       </c>
       <c r="E55" t="n">
-        <v>-2.745211267605633</v>
+        <v>0.3390410958904114</v>
       </c>
     </row>
     <row r="56">
@@ -1378,16 +1378,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.04267605633802816</v>
+        <v>-0.01417808219178082</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.001901408450704225</v>
+        <v>-0.014</v>
       </c>
       <c r="D56" t="n">
-        <v>-3.627464788732394</v>
+        <v>-0.1171232876712339</v>
       </c>
       <c r="E56" t="n">
-        <v>-3.627464788732394</v>
+        <v>-0.1171232876712339</v>
       </c>
     </row>
     <row r="57">
@@ -1395,16 +1395,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.04225352112676056</v>
+        <v>-0.01294520547945205</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.001901408450704225</v>
+        <v>-0.009999999999999998</v>
       </c>
       <c r="D57" t="n">
-        <v>-3.150422535211271</v>
+        <v>-0.2034246575342458</v>
       </c>
       <c r="E57" t="n">
-        <v>-3.150422535211271</v>
+        <v>-0.2034246575342458</v>
       </c>
     </row>
     <row r="58">
@@ -1412,16 +1412,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.04183098591549295</v>
+        <v>-0.01047945205479452</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.001056338028169014</v>
+        <v>-0.005999999999999999</v>
       </c>
       <c r="D58" t="n">
-        <v>-3.114507042253517</v>
+        <v>-1.485616438356165</v>
       </c>
       <c r="E58" t="n">
-        <v>-3.114507042253517</v>
+        <v>-1.485616438356165</v>
       </c>
     </row>
     <row r="59">
@@ -1429,16 +1429,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.04098591549295774</v>
+        <v>-0.008013698630136986</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.0002112676056338028</v>
+        <v>-0.0028</v>
       </c>
       <c r="D59" t="n">
-        <v>-2.601549295774647</v>
+        <v>-1.658219178082192</v>
       </c>
       <c r="E59" t="n">
-        <v>-2.601549295774647</v>
+        <v>-1.658219178082192</v>
       </c>
     </row>
     <row r="60">
@@ -1446,16 +1446,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.04014084507042253</v>
+        <v>-0.006780821917808219</v>
       </c>
       <c r="C60" t="n">
-        <v>0.0006338028169014084</v>
+        <v>0.0012</v>
       </c>
       <c r="D60" t="n">
-        <v>-2.529718309859154</v>
+        <v>-0.6349315068493151</v>
       </c>
       <c r="E60" t="n">
-        <v>-2.529718309859154</v>
+        <v>-0.6349315068493151</v>
       </c>
     </row>
     <row r="61">
@@ -1463,16 +1463,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.03929577464788732</v>
+        <v>-0.004315068493150684</v>
       </c>
       <c r="C61" t="n">
-        <v>0.001901408450704225</v>
+        <v>0.0032</v>
       </c>
       <c r="D61" t="n">
-        <v>-2.457887323943661</v>
+        <v>-1.917123287671233</v>
       </c>
       <c r="E61" t="n">
-        <v>-2.457887323943661</v>
+        <v>-1.917123287671233</v>
       </c>
     </row>
     <row r="62">
@@ -1480,16 +1480,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.03971830985915493</v>
+        <v>-0.002671232876712329</v>
       </c>
       <c r="C62" t="n">
-        <v>0.002323943661971831</v>
+        <v>0.005599999999999999</v>
       </c>
       <c r="D62" t="n">
-        <v>-3.817183098591553</v>
+        <v>-1.292465753424657</v>
       </c>
       <c r="E62" t="n">
-        <v>-3.817183098591553</v>
+        <v>-1.292465753424657</v>
       </c>
     </row>
     <row r="63">
@@ -1497,16 +1497,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.03887323943661972</v>
+        <v>-0.001027397260273973</v>
       </c>
       <c r="C63" t="n">
-        <v>0.003169014084507042</v>
+        <v>0.0072</v>
       </c>
       <c r="D63" t="n">
-        <v>-2.421971830985915</v>
+        <v>-1.407534246575342</v>
       </c>
       <c r="E63" t="n">
-        <v>-2.421971830985915</v>
+        <v>-1.407534246575342</v>
       </c>
     </row>
     <row r="64">
@@ -1514,16 +1514,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.0380281690140845</v>
+        <v>-0.0006164383561643835</v>
       </c>
       <c r="C64" t="n">
-        <v>0.004859154929577465</v>
+        <v>0.0092</v>
       </c>
       <c r="D64" t="n">
-        <v>-2.350140845070422</v>
+        <v>-0.3267123287671232</v>
       </c>
       <c r="E64" t="n">
-        <v>-2.350140845070422</v>
+        <v>-0.3267123287671232</v>
       </c>
     </row>
     <row r="65">
@@ -1531,16 +1531,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.03718309859154929</v>
+        <v>0.001027397260273973</v>
       </c>
       <c r="C65" t="n">
-        <v>0.005704225352112675</v>
+        <v>0.008799999999999999</v>
       </c>
       <c r="D65" t="n">
-        <v>-2.278309859154929</v>
+        <v>-1.551369863013699</v>
       </c>
       <c r="E65" t="n">
-        <v>-2.278309859154929</v>
+        <v>-1.551369863013699</v>
       </c>
     </row>
     <row r="66">
@@ -1548,16 +1548,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.03676056338028168</v>
+        <v>0.002671232876712329</v>
       </c>
       <c r="C66" t="n">
-        <v>0.006549295774647887</v>
+        <v>0.008799999999999999</v>
       </c>
       <c r="D66" t="n">
-        <v>-2.683521126760559</v>
+        <v>-1.666438356164383</v>
       </c>
       <c r="E66" t="n">
-        <v>-2.683521126760559</v>
+        <v>-1.666438356164383</v>
       </c>
     </row>
     <row r="67">
@@ -1565,16 +1565,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.03676056338028168</v>
+        <v>0.003082191780821918</v>
       </c>
       <c r="C67" t="n">
-        <v>0.006549295774647887</v>
+        <v>0.008799999999999999</v>
       </c>
       <c r="D67" t="n">
-        <v>-3.124647887323943</v>
+        <v>-0.5856164383561645</v>
       </c>
       <c r="E67" t="n">
-        <v>-3.124647887323943</v>
+        <v>-0.5856164383561645</v>
       </c>
     </row>
     <row r="68">
@@ -1582,16 +1582,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.0376056338028169</v>
+        <v>0.003493150684931506</v>
       </c>
       <c r="C68" t="n">
-        <v>0.006549295774647887</v>
+        <v>0.008</v>
       </c>
       <c r="D68" t="n">
-        <v>-4.078732394366197</v>
+        <v>-0.6143835616438353</v>
       </c>
       <c r="E68" t="n">
-        <v>-4.078732394366197</v>
+        <v>-0.6143835616438353</v>
       </c>
     </row>
     <row r="69">
@@ -1599,16 +1599,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.03845070422535211</v>
+        <v>0.003493150684931506</v>
       </c>
       <c r="C69" t="n">
-        <v>0.006549295774647887</v>
+        <v>0.0072</v>
       </c>
       <c r="D69" t="n">
-        <v>-4.15056338028169</v>
+        <v>-0.2445205479452054</v>
       </c>
       <c r="E69" t="n">
-        <v>-4.15056338028169</v>
+        <v>-0.2445205479452054</v>
       </c>
     </row>
     <row r="70">
@@ -1616,16 +1616,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.03929577464788732</v>
+        <v>0.003082191780821918</v>
       </c>
       <c r="C70" t="n">
-        <v>0.005704225352112675</v>
+        <v>0.005599999999999999</v>
       </c>
       <c r="D70" t="n">
-        <v>-4.222394366197182</v>
+        <v>0.1541095890410956</v>
       </c>
       <c r="E70" t="n">
-        <v>-4.222394366197182</v>
+        <v>0.1541095890410956</v>
       </c>
     </row>
     <row r="71">
@@ -1633,16 +1633,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.04056338028169014</v>
+        <v>0.002260273972602739</v>
       </c>
       <c r="C71" t="n">
-        <v>0.004859154929577465</v>
+        <v>0.004</v>
       </c>
       <c r="D71" t="n">
-        <v>-4.771267605633806</v>
+        <v>0.5815068493150688</v>
       </c>
       <c r="E71" t="n">
-        <v>-4.771267605633806</v>
+        <v>0.5815068493150688</v>
       </c>
     </row>
     <row r="72">
@@ -1650,16 +1650,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.04098591549295774</v>
+        <v>0.001438356164383561</v>
       </c>
       <c r="C72" t="n">
-        <v>0.004859154929577465</v>
+        <v>0.0016</v>
       </c>
       <c r="D72" t="n">
-        <v>-3.924929577464785</v>
+        <v>0.6390410958904108</v>
       </c>
       <c r="E72" t="n">
-        <v>-3.924929577464785</v>
+        <v>0.6390410958904108</v>
       </c>
     </row>
     <row r="73">
@@ -1667,16 +1667,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.04183098591549295</v>
+        <v>0.0006164383561643835</v>
       </c>
       <c r="C73" t="n">
-        <v>0.004014084507042253</v>
+        <v>-0.0004</v>
       </c>
       <c r="D73" t="n">
-        <v>-4.437887323943662</v>
+        <v>0.6965753424657533</v>
       </c>
       <c r="E73" t="n">
-        <v>-4.437887323943662</v>
+        <v>0.6965753424657533</v>
       </c>
     </row>
     <row r="74">
@@ -1684,16 +1684,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.04394366197183099</v>
+        <v>0.0002054794520547945</v>
       </c>
       <c r="C74" t="n">
-        <v>0.002323943661971831</v>
+        <v>-0.0028</v>
       </c>
       <c r="D74" t="n">
-        <v>-5.940845070422539</v>
+        <v>0.3554794520547945</v>
       </c>
       <c r="E74" t="n">
-        <v>-5.940845070422539</v>
+        <v>0.3554794520547945</v>
       </c>
     </row>
     <row r="75">
@@ -1701,16 +1701,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.0447887323943662</v>
+        <v>-0.001849315068493151</v>
       </c>
       <c r="C75" t="n">
-        <v>0.002323943661971831</v>
+        <v>-0.0052</v>
       </c>
       <c r="D75" t="n">
-        <v>-4.689295774647888</v>
+        <v>1.978767123287671</v>
       </c>
       <c r="E75" t="n">
-        <v>-4.689295774647888</v>
+        <v>1.978767123287671</v>
       </c>
     </row>
     <row r="76">
@@ -1718,16 +1718,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.04605633802816901</v>
+        <v>-0.002671232876712329</v>
       </c>
       <c r="C76" t="n">
-        <v>0.00147887323943662</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="D76" t="n">
-        <v>-5.238169014084503</v>
+        <v>0.9267123287671231</v>
       </c>
       <c r="E76" t="n">
-        <v>-5.238169014084503</v>
+        <v>0.9267123287671231</v>
       </c>
     </row>
     <row r="77">
@@ -1735,16 +1735,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.04690140845070422</v>
+        <v>-0.004726027397260274</v>
       </c>
       <c r="C77" t="n">
-        <v>0.0006338028169014084</v>
+        <v>-0.0108</v>
       </c>
       <c r="D77" t="n">
-        <v>-4.86887323943662</v>
+        <v>2.18013698630137</v>
       </c>
       <c r="E77" t="n">
-        <v>-4.86887323943662</v>
+        <v>2.18013698630137</v>
       </c>
     </row>
     <row r="78">
@@ -1752,16 +1752,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.04774647887323943</v>
+        <v>-0.005547945205479451</v>
       </c>
       <c r="C78" t="n">
-        <v>0.0006338028169014084</v>
+        <v>-0.0136</v>
       </c>
       <c r="D78" t="n">
-        <v>-4.940704225352112</v>
+        <v>1.128082191780821</v>
       </c>
       <c r="E78" t="n">
-        <v>-4.940704225352112</v>
+        <v>1.128082191780821</v>
       </c>
     </row>
     <row r="79">
@@ -1769,16 +1769,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.04774647887323943</v>
+        <v>-0.007191780821917807</v>
       </c>
       <c r="C79" t="n">
-        <v>0.0006338028169014084</v>
+        <v>-0.016</v>
       </c>
       <c r="D79" t="n">
-        <v>-4.058450704225351</v>
+        <v>1.982876712328767</v>
       </c>
       <c r="E79" t="n">
-        <v>-4.058450704225351</v>
+        <v>1.982876712328767</v>
       </c>
     </row>
     <row r="80">
@@ -1786,16 +1786,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.04859154929577465</v>
+        <v>-0.008835616438356163</v>
       </c>
       <c r="C80" t="n">
-        <v>0.0002112676056338028</v>
+        <v>-0.0176</v>
       </c>
       <c r="D80" t="n">
-        <v>-5.012535211267606</v>
+        <v>2.097945205479451</v>
       </c>
       <c r="E80" t="n">
-        <v>-5.012535211267606</v>
+        <v>2.097945205479451</v>
       </c>
     </row>
     <row r="81">
@@ -1803,16 +1803,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.04859154929577465</v>
+        <v>-0.009246575342465754</v>
       </c>
       <c r="C81" t="n">
-        <v>0.00147887323943662</v>
+        <v>-0.0192</v>
       </c>
       <c r="D81" t="n">
-        <v>-4.130281690140845</v>
+        <v>1.017123287671234</v>
       </c>
       <c r="E81" t="n">
-        <v>-4.130281690140845</v>
+        <v>1.017123287671234</v>
       </c>
     </row>
     <row r="82">
@@ -1820,16 +1820,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.04943661971830986</v>
+        <v>-0.01006849315068493</v>
       </c>
       <c r="C82" t="n">
-        <v>0.001901408450704225</v>
+        <v>-0.02</v>
       </c>
       <c r="D82" t="n">
-        <v>-5.084366197183098</v>
+        <v>1.444520547945205</v>
       </c>
       <c r="E82" t="n">
-        <v>-5.084366197183098</v>
+        <v>1.444520547945205</v>
       </c>
     </row>
     <row r="83">
@@ -1837,16 +1837,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.04943661971830986</v>
+        <v>-0.01089041095890411</v>
       </c>
       <c r="C83" t="n">
-        <v>0.002746478873239437</v>
+        <v>-0.0208</v>
       </c>
       <c r="D83" t="n">
-        <v>-4.202112676056338</v>
+        <v>1.502054794520547</v>
       </c>
       <c r="E83" t="n">
-        <v>-4.202112676056338</v>
+        <v>1.502054794520547</v>
       </c>
     </row>
     <row r="84">
@@ -1854,16 +1854,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.04985915492957746</v>
+        <v>-0.01171232876712329</v>
       </c>
       <c r="C84" t="n">
-        <v>0.003591549295774648</v>
+        <v>-0.0216</v>
       </c>
       <c r="D84" t="n">
-        <v>-4.679154929577461</v>
+        <v>1.55958904109589</v>
       </c>
       <c r="E84" t="n">
-        <v>-4.679154929577461</v>
+        <v>1.55958904109589</v>
       </c>
     </row>
     <row r="85">
@@ -1871,16 +1871,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.04901408450704225</v>
+        <v>-0.01253424657534247</v>
       </c>
       <c r="C85" t="n">
-        <v>0.005704225352112675</v>
+        <v>-0.0208</v>
       </c>
       <c r="D85" t="n">
-        <v>-3.28394366197183</v>
+        <v>1.617123287671234</v>
       </c>
       <c r="E85" t="n">
-        <v>-3.28394366197183</v>
+        <v>1.617123287671234</v>
       </c>
     </row>
     <row r="86">
@@ -1888,16 +1888,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.04901408450704225</v>
+        <v>-0.01294520547945205</v>
       </c>
       <c r="C86" t="n">
-        <v>0.007394366197183098</v>
+        <v>-0.0196</v>
       </c>
       <c r="D86" t="n">
-        <v>-4.166197183098591</v>
+        <v>1.276027397260274</v>
       </c>
       <c r="E86" t="n">
-        <v>-4.166197183098591</v>
+        <v>1.276027397260274</v>
       </c>
     </row>
     <row r="87">
@@ -1905,16 +1905,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.04816901408450704</v>
+        <v>-0.01212328767123288</v>
       </c>
       <c r="C87" t="n">
-        <v>0.00908450704225352</v>
+        <v>-0.0192</v>
       </c>
       <c r="D87" t="n">
-        <v>-3.212112676056337</v>
+        <v>0.1089041095890416</v>
       </c>
       <c r="E87" t="n">
-        <v>-3.212112676056337</v>
+        <v>0.1089041095890416</v>
       </c>
     </row>
     <row r="88">
@@ -1922,16 +1922,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.04816901408450704</v>
+        <v>-0.01253424657534247</v>
       </c>
       <c r="C88" t="n">
-        <v>0.01035211267605634</v>
+        <v>-0.0168</v>
       </c>
       <c r="D88" t="n">
-        <v>-4.094366197183098</v>
+        <v>1.247260273972602</v>
       </c>
       <c r="E88" t="n">
-        <v>-4.094366197183098</v>
+        <v>1.247260273972602</v>
       </c>
     </row>
     <row r="89">
@@ -1939,16 +1939,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.04690140845070422</v>
+        <v>-0.01171232876712329</v>
       </c>
       <c r="C89" t="n">
-        <v>0.01246478873239436</v>
+        <v>-0.0152</v>
       </c>
       <c r="D89" t="n">
-        <v>-2.663239436619722</v>
+        <v>0.08013698630136867</v>
       </c>
       <c r="E89" t="n">
-        <v>-2.663239436619722</v>
+        <v>0.08013698630136867</v>
       </c>
     </row>
     <row r="90">
@@ -1956,16 +1956,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.04605633802816901</v>
+        <v>-0.01089041095890411</v>
       </c>
       <c r="C90" t="n">
-        <v>0.01330985915492958</v>
+        <v>-0.0132</v>
       </c>
       <c r="D90" t="n">
-        <v>-3.032535211267605</v>
+        <v>0.02260273972602778</v>
       </c>
       <c r="E90" t="n">
-        <v>-3.032535211267605</v>
+        <v>0.02260273972602778</v>
       </c>
     </row>
     <row r="91">
@@ -1973,16 +1973,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.04605633802816901</v>
+        <v>-0.009657534246575342</v>
       </c>
       <c r="C91" t="n">
-        <v>0.01373239436619718</v>
+        <v>-0.0108</v>
       </c>
       <c r="D91" t="n">
-        <v>-3.914788732394366</v>
+        <v>-0.4335616438356156</v>
       </c>
       <c r="E91" t="n">
-        <v>-3.914788732394366</v>
+        <v>-0.4335616438356156</v>
       </c>
     </row>
     <row r="92">
@@ -1990,16 +1990,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.0452112676056338</v>
+        <v>-0.01006849315068493</v>
       </c>
       <c r="C92" t="n">
-        <v>0.01415492957746479</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="D92" t="n">
-        <v>-2.960704225352112</v>
+        <v>1.074657534246575</v>
       </c>
       <c r="E92" t="n">
-        <v>-2.960704225352112</v>
+        <v>1.074657534246575</v>
       </c>
     </row>
     <row r="93">
@@ -2007,16 +2007,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.04436619718309859</v>
+        <v>-0.008835616438356163</v>
       </c>
       <c r="C93" t="n">
-        <v>0.01330985915492958</v>
+        <v>-0.005599999999999999</v>
       </c>
       <c r="D93" t="n">
-        <v>-2.888873239436619</v>
+        <v>-0.4910958904109599</v>
       </c>
       <c r="E93" t="n">
-        <v>-2.888873239436619</v>
+        <v>-0.4910958904109599</v>
       </c>
     </row>
     <row r="94">
@@ -2024,16 +2024,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.04436619718309859</v>
+        <v>-0.008013698630136986</v>
       </c>
       <c r="C94" t="n">
-        <v>0.01161971830985915</v>
+        <v>-0.0036</v>
       </c>
       <c r="D94" t="n">
-        <v>-3.77112676056338</v>
+        <v>-0.1787671232876707</v>
       </c>
       <c r="E94" t="n">
-        <v>-3.77112676056338</v>
+        <v>-0.1787671232876707</v>
       </c>
     </row>
     <row r="95">
@@ -2041,16 +2041,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.04436619718309859</v>
+        <v>-0.006780821917808219</v>
       </c>
       <c r="C95" t="n">
-        <v>0.009507042253521126</v>
+        <v>-0.002</v>
       </c>
       <c r="D95" t="n">
-        <v>-3.77112676056338</v>
+        <v>-0.6349315068493151</v>
       </c>
       <c r="E95" t="n">
-        <v>-3.77112676056338</v>
+        <v>-0.6349315068493151</v>
       </c>
     </row>
     <row r="96">
@@ -2058,16 +2058,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.04352112676056338</v>
+        <v>-0.005136986301369863</v>
       </c>
       <c r="C96" t="n">
-        <v>0.008239436619718309</v>
+        <v>-0.0012</v>
       </c>
       <c r="D96" t="n">
-        <v>-2.817042253521126</v>
+        <v>-1.11986301369863</v>
       </c>
       <c r="E96" t="n">
-        <v>-2.817042253521126</v>
+        <v>-1.11986301369863</v>
       </c>
     </row>
     <row r="97">
@@ -2075,16 +2075,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.04352112676056338</v>
+        <v>-0.003493150684931506</v>
       </c>
       <c r="C97" t="n">
-        <v>0.005704225352112675</v>
+        <v>-0.0004</v>
       </c>
       <c r="D97" t="n">
-        <v>-3.699295774647887</v>
+        <v>-1.234931506849315</v>
       </c>
       <c r="E97" t="n">
-        <v>-3.699295774647887</v>
+        <v>-1.234931506849315</v>
       </c>
     </row>
     <row r="98">
@@ -2092,16 +2092,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.04352112676056338</v>
+        <v>-0.001849315068493151</v>
       </c>
       <c r="C98" t="n">
-        <v>0.003169014084507042</v>
+        <v>-0.0007999999999999999</v>
       </c>
       <c r="D98" t="n">
-        <v>-3.699295774647887</v>
+        <v>-1.35</v>
       </c>
       <c r="E98" t="n">
-        <v>-3.699295774647887</v>
+        <v>-1.35</v>
       </c>
     </row>
     <row r="99">
@@ -2109,16 +2109,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.04352112676056338</v>
+        <v>-0.001027397260273973</v>
       </c>
       <c r="C99" t="n">
-        <v>0.0006338028169014084</v>
+        <v>-0.0016</v>
       </c>
       <c r="D99" t="n">
-        <v>-3.699295774647887</v>
+        <v>-0.6678082191780823</v>
       </c>
       <c r="E99" t="n">
-        <v>-3.699295774647887</v>
+        <v>-0.6678082191780823</v>
       </c>
     </row>
     <row r="100">
@@ -2126,16 +2126,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.04436619718309859</v>
+        <v>-0.0002054794520547945</v>
       </c>
       <c r="C100" t="n">
-        <v>-0.001901408450704225</v>
+        <v>-0.0016</v>
       </c>
       <c r="D100" t="n">
-        <v>-4.653380281690141</v>
+        <v>-0.7253424657534246</v>
       </c>
       <c r="E100" t="n">
-        <v>-4.653380281690141</v>
+        <v>-0.7253424657534246</v>
       </c>
     </row>
     <row r="101">
@@ -2143,16 +2143,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.04436619718309859</v>
+        <v>0.0006164383561643835</v>
       </c>
       <c r="C101" t="n">
-        <v>-0.003591549295774648</v>
+        <v>-0.0032</v>
       </c>
       <c r="D101" t="n">
-        <v>-3.77112676056338</v>
+        <v>-0.7828767123287671</v>
       </c>
       <c r="E101" t="n">
-        <v>-3.77112676056338</v>
+        <v>-0.7828767123287671</v>
       </c>
     </row>
     <row r="102">
@@ -2160,16 +2160,16 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>0.0447887323943662</v>
+        <v>0.001849315068493151</v>
       </c>
       <c r="C102" t="n">
-        <v>-0.00528169014084507</v>
+        <v>-0.0048</v>
       </c>
       <c r="D102" t="n">
-        <v>-4.248169014084511</v>
+        <v>-1.239041095890411</v>
       </c>
       <c r="E102" t="n">
-        <v>-4.248169014084511</v>
+        <v>-1.239041095890411</v>
       </c>
     </row>
     <row r="103">
@@ -2177,16 +2177,16 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>0.04352112676056338</v>
+        <v>0.002260273972602739</v>
       </c>
       <c r="C103" t="n">
-        <v>-0.00528169014084507</v>
+        <v>-0.006399999999999999</v>
       </c>
       <c r="D103" t="n">
-        <v>-2.375915492957742</v>
+        <v>-0.5280821917808216</v>
       </c>
       <c r="E103" t="n">
-        <v>-2.375915492957742</v>
+        <v>-0.5280821917808216</v>
       </c>
     </row>
     <row r="104">
@@ -2194,16 +2194,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.04309859154929577</v>
+        <v>0.002260273972602739</v>
       </c>
       <c r="C104" t="n">
-        <v>-0.006126760563380281</v>
+        <v>-0.008</v>
       </c>
       <c r="D104" t="n">
-        <v>-3.222253521126764</v>
+        <v>-0.1582191780821918</v>
       </c>
       <c r="E104" t="n">
-        <v>-3.222253521126764</v>
+        <v>-0.1582191780821918</v>
       </c>
     </row>
     <row r="105">
@@ -2211,16 +2211,16 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.04098591549295774</v>
+        <v>0.002671232876712329</v>
       </c>
       <c r="C105" t="n">
-        <v>-0.004859154929577465</v>
+        <v>-0.009999999999999998</v>
       </c>
       <c r="D105" t="n">
-        <v>-1.278169014084503</v>
+        <v>-0.5568493150684932</v>
       </c>
       <c r="E105" t="n">
-        <v>-1.278169014084503</v>
+        <v>-0.5568493150684932</v>
       </c>
     </row>
     <row r="106">
@@ -2228,16 +2228,16 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.04056338028169014</v>
+        <v>0.003082191780821918</v>
       </c>
       <c r="C106" t="n">
-        <v>-0.00528169014084507</v>
+        <v>-0.0116</v>
       </c>
       <c r="D106" t="n">
-        <v>-3.006760563380285</v>
+        <v>-0.5856164383561645</v>
       </c>
       <c r="E106" t="n">
-        <v>-3.006760563380285</v>
+        <v>-0.5856164383561645</v>
       </c>
     </row>
     <row r="107">
@@ -2245,16 +2245,16 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.03887323943661972</v>
+        <v>0.001849315068493151</v>
       </c>
       <c r="C107" t="n">
-        <v>-0.004014084507042253</v>
+        <v>-0.0124</v>
       </c>
       <c r="D107" t="n">
-        <v>-1.539718309859155</v>
+        <v>0.9801369863013698</v>
       </c>
       <c r="E107" t="n">
-        <v>-1.539718309859155</v>
+        <v>0.9801369863013698</v>
       </c>
     </row>
     <row r="108">
@@ -2262,16 +2262,16 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.03676056338028168</v>
+        <v>0.001027397260273973</v>
       </c>
       <c r="C108" t="n">
-        <v>-0.002323943661971831</v>
+        <v>-0.014</v>
       </c>
       <c r="D108" t="n">
-        <v>-0.9190140845070376</v>
+        <v>0.6678082191780823</v>
       </c>
       <c r="E108" t="n">
-        <v>-0.9190140845070376</v>
+        <v>0.6678082191780823</v>
       </c>
     </row>
     <row r="109">
@@ -2279,16 +2279,16 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0.03549295774647887</v>
+        <v>0.0006164383561643835</v>
       </c>
       <c r="C109" t="n">
-        <v>-0.00147887323943662</v>
+        <v>-0.0156</v>
       </c>
       <c r="D109" t="n">
-        <v>-1.693521126760567</v>
+        <v>0.3267123287671232</v>
       </c>
       <c r="E109" t="n">
-        <v>-1.693521126760567</v>
+        <v>0.3267123287671232</v>
       </c>
     </row>
     <row r="110">
@@ -2296,16 +2296,16 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>0.03338028169014085</v>
+        <v>-0.001027397260273973</v>
       </c>
       <c r="C110" t="n">
-        <v>0.0002112676056338028</v>
+        <v>-0.016</v>
       </c>
       <c r="D110" t="n">
-        <v>-0.6316901408450737</v>
+        <v>1.551369863013699</v>
       </c>
       <c r="E110" t="n">
-        <v>-0.6316901408450737</v>
+        <v>1.551369863013699</v>
       </c>
     </row>
     <row r="111">
@@ -2313,16 +2313,16 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>0.03295774647887324</v>
+        <v>-0.001849315068493151</v>
       </c>
       <c r="C111" t="n">
-        <v>0.0006338028169014084</v>
+        <v>-0.0168</v>
       </c>
       <c r="D111" t="n">
-        <v>-2.360281690140841</v>
+        <v>0.8691780821917809</v>
       </c>
       <c r="E111" t="n">
-        <v>-2.360281690140841</v>
+        <v>0.8691780821917809</v>
       </c>
     </row>
     <row r="112">
@@ -2330,16 +2330,16 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>0.03169014084507042</v>
+        <v>-0.002671232876712329</v>
       </c>
       <c r="C112" t="n">
-        <v>0.002323943661971831</v>
+        <v>-0.0172</v>
       </c>
       <c r="D112" t="n">
-        <v>-1.370281690140849</v>
+        <v>0.9267123287671231</v>
       </c>
       <c r="E112" t="n">
-        <v>-1.370281690140849</v>
+        <v>0.9267123287671231</v>
       </c>
     </row>
     <row r="113">
@@ -2347,16 +2347,16 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>0.03126760563380281</v>
+        <v>-0.004726027397260274</v>
       </c>
       <c r="C113" t="n">
-        <v>0.003169014084507042</v>
+        <v>-0.0168</v>
       </c>
       <c r="D113" t="n">
-        <v>-2.216619718309855</v>
+        <v>2.18013698630137</v>
       </c>
       <c r="E113" t="n">
-        <v>-2.216619718309855</v>
+        <v>2.18013698630137</v>
       </c>
     </row>
     <row r="114">
@@ -2364,16 +2364,16 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>0.0304225352112676</v>
+        <v>-0.005136986301369863</v>
       </c>
       <c r="C114" t="n">
-        <v>0.004436619718309859</v>
+        <v>-0.0168</v>
       </c>
       <c r="D114" t="n">
-        <v>-1.703661971830989</v>
+        <v>0.7294520547945202</v>
       </c>
       <c r="E114" t="n">
-        <v>-1.703661971830989</v>
+        <v>0.7294520547945202</v>
       </c>
     </row>
     <row r="115">
@@ -2381,16 +2381,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>0.03</v>
+        <v>-0.005547945205479451</v>
       </c>
       <c r="C115" t="n">
-        <v>0.00528169014084507</v>
+        <v>-0.0164</v>
       </c>
       <c r="D115" t="n">
-        <v>-2.108873239436619</v>
+        <v>0.7582191780821914</v>
       </c>
       <c r="E115" t="n">
-        <v>-2.108873239436619</v>
+        <v>0.7582191780821914</v>
       </c>
     </row>
     <row r="116">
@@ -2398,16 +2398,16 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0.03084507042253521</v>
+        <v>-0.008013698630136986</v>
       </c>
       <c r="C116" t="n">
-        <v>0.004859154929577465</v>
+        <v>-0.0148</v>
       </c>
       <c r="D116" t="n">
-        <v>-3.504084507042254</v>
+        <v>2.78013698630137</v>
       </c>
       <c r="E116" t="n">
-        <v>-3.504084507042254</v>
+        <v>2.78013698630137</v>
       </c>
     </row>
     <row r="117">
@@ -2415,16 +2415,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>0.03084507042253521</v>
+        <v>-0.008013698630136986</v>
       </c>
       <c r="C117" t="n">
-        <v>0.00528169014084507</v>
+        <v>-0.014</v>
       </c>
       <c r="D117" t="n">
-        <v>-2.621830985915493</v>
+        <v>0.560958904109589</v>
       </c>
       <c r="E117" t="n">
-        <v>-2.621830985915493</v>
+        <v>0.560958904109589</v>
       </c>
     </row>
     <row r="118">
@@ -2432,16 +2432,16 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0.03169014084507042</v>
+        <v>-0.008424657534246574</v>
       </c>
       <c r="C118" t="n">
-        <v>0.00528169014084507</v>
+        <v>-0.0124</v>
       </c>
       <c r="D118" t="n">
-        <v>-3.575915492957747</v>
+        <v>0.95958904109589</v>
       </c>
       <c r="E118" t="n">
-        <v>-3.575915492957747</v>
+        <v>0.95958904109589</v>
       </c>
     </row>
     <row r="119">
@@ -2449,16 +2449,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>0.03380281690140845</v>
+        <v>-0.008424657534246574</v>
       </c>
       <c r="C119" t="n">
-        <v>0.004014084507042253</v>
+        <v>-0.0116</v>
       </c>
       <c r="D119" t="n">
-        <v>-5.078873239436616</v>
+        <v>0.5897260273972602</v>
       </c>
       <c r="E119" t="n">
-        <v>-5.078873239436616</v>
+        <v>0.5897260273972602</v>
       </c>
     </row>
     <row r="120">
@@ -2466,16 +2466,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>0.03507042253521127</v>
+        <v>-0.008424657534246574</v>
       </c>
       <c r="C120" t="n">
-        <v>0.004014084507042253</v>
+        <v>-0.009999999999999998</v>
       </c>
       <c r="D120" t="n">
-        <v>-4.304366197183103</v>
+        <v>0.5897260273972602</v>
       </c>
       <c r="E120" t="n">
-        <v>-4.304366197183103</v>
+        <v>0.5897260273972602</v>
       </c>
     </row>
     <row r="121">
@@ -2483,16 +2483,16 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>0.03676056338028168</v>
+        <v>-0.008424657534246574</v>
       </c>
       <c r="C121" t="n">
-        <v>0.003591549295774648</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="D121" t="n">
-        <v>-4.889154929577458</v>
+        <v>0.5897260273972602</v>
       </c>
       <c r="E121" t="n">
-        <v>-4.889154929577458</v>
+        <v>0.5897260273972602</v>
       </c>
     </row>
     <row r="122">
@@ -2500,16 +2500,16 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>0.03845070422535211</v>
+        <v>-0.008013698630136986</v>
       </c>
       <c r="C122" t="n">
-        <v>0.002746478873239437</v>
+        <v>-0.0068</v>
       </c>
       <c r="D122" t="n">
-        <v>-5.032816901408451</v>
+        <v>0.1910958904109591</v>
       </c>
       <c r="E122" t="n">
-        <v>-5.032816901408451</v>
+        <v>0.1910958904109591</v>
       </c>
     </row>
     <row r="123">
@@ -2517,16 +2517,16 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>0.04098591549295774</v>
+        <v>-0.00636986301369863</v>
       </c>
       <c r="C123" t="n">
-        <v>0.001901408450704225</v>
+        <v>-0.0052</v>
       </c>
       <c r="D123" t="n">
-        <v>-6.13056338028169</v>
+        <v>-1.033561643835616</v>
       </c>
       <c r="E123" t="n">
-        <v>-6.13056338028169</v>
+        <v>-1.033561643835616</v>
       </c>
     </row>
     <row r="124">
@@ -2534,16 +2534,16 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>0.04352112676056338</v>
+        <v>-0.005958904109589041</v>
       </c>
       <c r="C124" t="n">
-        <v>0.001901408450704225</v>
+        <v>-0.004399999999999999</v>
       </c>
       <c r="D124" t="n">
-        <v>-6.346056338028169</v>
+        <v>0.04726027397260296</v>
       </c>
       <c r="E124" t="n">
-        <v>-6.346056338028169</v>
+        <v>0.04726027397260296</v>
       </c>
     </row>
     <row r="125">
@@ -2551,16 +2551,16 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>0.0452112676056338</v>
+        <v>-0.003904109589041096</v>
       </c>
       <c r="C125" t="n">
-        <v>0.001056338028169014</v>
+        <v>-0.0036</v>
       </c>
       <c r="D125" t="n">
-        <v>-5.607464788732394</v>
+        <v>-1.576027397260274</v>
       </c>
       <c r="E125" t="n">
-        <v>-5.607464788732394</v>
+        <v>-1.576027397260274</v>
       </c>
     </row>
     <row r="126">
@@ -2568,16 +2568,16 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>0.04690140845070422</v>
+        <v>-0.003082191780821918</v>
       </c>
       <c r="C126" t="n">
-        <v>0.0006338028169014084</v>
+        <v>-0.0028</v>
       </c>
       <c r="D126" t="n">
-        <v>-5.75112676056338</v>
+        <v>-0.5239726027397259</v>
       </c>
       <c r="E126" t="n">
-        <v>-5.75112676056338</v>
+        <v>-0.5239726027397259</v>
       </c>
     </row>
     <row r="127">
@@ -2585,16 +2585,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>0.04774647887323943</v>
+        <v>-0.001849315068493151</v>
       </c>
       <c r="C127" t="n">
-        <v>-0.0002112676056338028</v>
+        <v>-0.002</v>
       </c>
       <c r="D127" t="n">
-        <v>-4.940704225352112</v>
+        <v>-0.9801369863013698</v>
       </c>
       <c r="E127" t="n">
-        <v>-4.940704225352112</v>
+        <v>-0.9801369863013698</v>
       </c>
     </row>
     <row r="128">
@@ -2602,16 +2602,16 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>0.04774647887323943</v>
+        <v>-0.0002054794520547945</v>
       </c>
       <c r="C128" t="n">
-        <v>-0.0002112676056338028</v>
+        <v>-0.0024</v>
       </c>
       <c r="D128" t="n">
-        <v>-4.058450704225351</v>
+        <v>-1.465068493150685</v>
       </c>
       <c r="E128" t="n">
-        <v>-4.058450704225351</v>
+        <v>-1.465068493150685</v>
       </c>
     </row>
     <row r="129">
@@ -2619,16 +2619,16 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>0.0456338028169014</v>
+        <v>0.001438356164383561</v>
       </c>
       <c r="C129" t="n">
-        <v>-0.0006338028169014084</v>
+        <v>-0.002</v>
       </c>
       <c r="D129" t="n">
-        <v>-1.673239436619713</v>
+        <v>-1.58013698630137</v>
       </c>
       <c r="E129" t="n">
-        <v>-1.673239436619713</v>
+        <v>-1.58013698630137</v>
       </c>
     </row>
     <row r="130">
@@ -2636,16 +2636,16 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>0.0376056338028169</v>
+        <v>0.003082191780821918</v>
       </c>
       <c r="C130" t="n">
-        <v>-0.004436619718309859</v>
+        <v>-0.002</v>
       </c>
       <c r="D130" t="n">
-        <v>5.184929577464788</v>
+        <v>-1.695205479452055</v>
       </c>
       <c r="E130" t="n">
-        <v>5.184929577464788</v>
+        <v>-1.695205479452055</v>
       </c>
     </row>
     <row r="131">
@@ -2653,16 +2653,16 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>0.02492957746478873</v>
+        <v>0.004726027397260274</v>
       </c>
       <c r="C131" t="n">
-        <v>-0.01246478873239436</v>
+        <v>-0.0032</v>
       </c>
       <c r="D131" t="n">
-        <v>11.11478873239436</v>
+        <v>-1.81027397260274</v>
       </c>
       <c r="E131" t="n">
-        <v>11.11478873239436</v>
+        <v>-1.81027397260274</v>
       </c>
     </row>
     <row r="132">
@@ -2670,16 +2670,16 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>0.008873239436619718</v>
+        <v>0.005547945205479451</v>
       </c>
       <c r="C132" t="n">
-        <v>-0.02387323943661972</v>
+        <v>-0.004</v>
       </c>
       <c r="D132" t="n">
-        <v>16.00859154929577</v>
+        <v>-1.128082191780821</v>
       </c>
       <c r="E132" t="n">
-        <v>16.00859154929577</v>
+        <v>-1.128082191780821</v>
       </c>
     </row>
     <row r="133">
@@ -2687,16 +2687,16 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>-0.01014084507042253</v>
+        <v>0.005547945205479451</v>
       </c>
       <c r="C133" t="n">
-        <v>-0.03739436619718309</v>
+        <v>-0.0048</v>
       </c>
       <c r="D133" t="n">
-        <v>20.71267605633803</v>
+        <v>-0.3883561643835616</v>
       </c>
       <c r="E133" t="n">
-        <v>20.71267605633803</v>
+        <v>-0.3883561643835616</v>
       </c>
     </row>
     <row r="134">
@@ -2704,16 +2704,16 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>-0.03211267605633802</v>
+        <v>0.005547945205479451</v>
       </c>
       <c r="C134" t="n">
-        <v>-0.05133802816901408</v>
+        <v>-0.005599999999999999</v>
       </c>
       <c r="D134" t="n">
-        <v>25.6681690140845</v>
+        <v>-0.3883561643835616</v>
       </c>
       <c r="E134" t="n">
-        <v>25.6681690140845</v>
+        <v>-0.3883561643835616</v>
       </c>
     </row>
     <row r="135">
@@ -2721,16 +2721,16 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>-0.05619718309859154</v>
+        <v>0.004726027397260274</v>
       </c>
       <c r="C135" t="n">
-        <v>-0.06654929577464788</v>
+        <v>-0.0068</v>
       </c>
       <c r="D135" t="n">
-        <v>29.92098591549296</v>
+        <v>0.4089041095890406</v>
       </c>
       <c r="E135" t="n">
-        <v>29.92098591549296</v>
+        <v>0.4089041095890406</v>
       </c>
     </row>
     <row r="136">
@@ -2738,16 +2738,16 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>-0.08154929577464788</v>
+        <v>0.003904109589041096</v>
       </c>
       <c r="C136" t="n">
-        <v>-0.0830281690140845</v>
+        <v>-0.007599999999999999</v>
       </c>
       <c r="D136" t="n">
-        <v>33.39929577464788</v>
+        <v>0.4664383561643839</v>
       </c>
       <c r="E136" t="n">
-        <v>33.39929577464788</v>
+        <v>0.4664383561643839</v>
       </c>
     </row>
     <row r="137">
@@ -2755,16 +2755,16 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>0.06760563380281689</v>
+        <v>0.003493150684931506</v>
       </c>
       <c r="C137" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.009599999999999999</v>
       </c>
       <c r="D137" t="n">
-        <v>-187.0495774647887</v>
+        <v>0.1253424657534248</v>
       </c>
       <c r="E137" t="n">
-        <v>-187.0495774647887</v>
+        <v>0.1253424657534248</v>
       </c>
     </row>
     <row r="138">
@@ -2772,16 +2772,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>0.07521126760563379</v>
+        <v>0.001849315068493151</v>
       </c>
       <c r="C138" t="n">
-        <v>0.1417605633802817</v>
+        <v>-0.009999999999999998</v>
       </c>
       <c r="D138" t="n">
-        <v>-216.8104225352112</v>
+        <v>1.35</v>
       </c>
       <c r="E138" t="n">
-        <v>-216.8104225352112</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="139">
@@ -2789,16 +2789,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>0.08830985915492957</v>
+        <v>0.0006164383561643835</v>
       </c>
       <c r="C139" t="n">
-        <v>0.1413380281690141</v>
+        <v>-0.0112</v>
       </c>
       <c r="D139" t="n">
-        <v>-249.6849295774648</v>
+        <v>1.066438356164384</v>
       </c>
       <c r="E139" t="n">
-        <v>-249.6849295774648</v>
+        <v>1.066438356164384</v>
       </c>
     </row>
     <row r="140">
@@ -2806,16 +2806,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0.1001408450704225</v>
+        <v>-0.001027397260273973</v>
       </c>
       <c r="C140" t="n">
-        <v>0.1413380281690141</v>
+        <v>-0.012</v>
       </c>
       <c r="D140" t="n">
-        <v>-20.86352112676055</v>
+        <v>1.551369863013699</v>
       </c>
       <c r="E140" t="n">
-        <v>-20.86352112676055</v>
+        <v>1.551369863013699</v>
       </c>
     </row>
     <row r="141">
@@ -2823,16 +2823,16 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>0.1170422535211268</v>
+        <v>-0.002671232876712329</v>
       </c>
       <c r="C141" t="n">
-        <v>0.1426056338028169</v>
+        <v>-0.0128</v>
       </c>
       <c r="D141" t="n">
-        <v>-27.59366197183099</v>
+        <v>1.666438356164383</v>
       </c>
       <c r="E141" t="n">
-        <v>-27.59366197183099</v>
+        <v>1.666438356164383</v>
       </c>
     </row>
     <row r="142">
@@ -2840,16 +2840,16 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>0.1170422535211268</v>
+        <v>-0.003904109589041096</v>
       </c>
       <c r="C142" t="n">
-        <v>0.1426056338028169</v>
+        <v>-0.0132</v>
       </c>
       <c r="D142" t="n">
-        <v>-27.59366197183099</v>
+        <v>1.382876712328767</v>
       </c>
       <c r="E142" t="n">
-        <v>-27.59366197183099</v>
+        <v>1.382876712328767</v>
       </c>
     </row>
     <row r="143">
@@ -2857,16 +2857,16 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>-0.1457746478873239</v>
+        <v>-0.005136986301369863</v>
       </c>
       <c r="C143" t="n">
-        <v>-0.1045774647887324</v>
+        <v>-0.0128</v>
       </c>
       <c r="D143" t="n">
-        <v>286.7716901408451</v>
+        <v>1.469178082191781</v>
       </c>
       <c r="E143" t="n">
-        <v>286.7716901408451</v>
+        <v>1.469178082191781</v>
       </c>
     </row>
     <row r="144">
@@ -2874,16 +2874,16 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>-0.1428169014084507</v>
+        <v>-0.006780821917808219</v>
       </c>
       <c r="C144" t="n">
-        <v>-0.1075352112676056</v>
+        <v>-0.0128</v>
       </c>
       <c r="D144" t="n">
-        <v>9.051549295774628</v>
+        <v>1.954109589041096</v>
       </c>
       <c r="E144" t="n">
-        <v>9.051549295774628</v>
+        <v>1.954109589041096</v>
       </c>
     </row>
     <row r="145">
@@ -2891,16 +2891,16 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>-0.152112676056338</v>
+        <v>-0.007602739726027397</v>
       </c>
       <c r="C145" t="n">
-        <v>-0.01373239436619718</v>
+        <v>-0.0124</v>
       </c>
       <c r="D145" t="n">
-        <v>34.54478873239435</v>
+        <v>1.271917808219178</v>
       </c>
       <c r="E145" t="n">
-        <v>34.54478873239435</v>
+        <v>1.271917808219178</v>
       </c>
     </row>
     <row r="146">
@@ -2908,16 +2908,16 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>-0.163943661971831</v>
+        <v>-0.009246575342465754</v>
       </c>
       <c r="C146" t="n">
-        <v>-0.008661971830985915</v>
+        <v>-0.0112</v>
       </c>
       <c r="D146" t="n">
-        <v>39.52056338028169</v>
+        <v>2.126712328767124</v>
       </c>
       <c r="E146" t="n">
-        <v>39.52056338028169</v>
+        <v>2.126712328767124</v>
       </c>
     </row>
     <row r="147">
@@ -2925,16 +2925,16 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>-0.1635211267605634</v>
+        <v>-0.01006849315068493</v>
       </c>
       <c r="C147" t="n">
-        <v>-0.008661971830985915</v>
+        <v>-0.0104</v>
       </c>
       <c r="D147" t="n">
-        <v>41.24915492957748</v>
+        <v>1.444520547945205</v>
       </c>
       <c r="E147" t="n">
-        <v>41.24915492957748</v>
+        <v>1.444520547945205</v>
       </c>
     </row>
     <row r="148">
@@ -2942,16 +2942,16 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>-0.1635211267605634</v>
+        <v>-0.01006849315068493</v>
       </c>
       <c r="C148" t="n">
-        <v>-0.008661971830985915</v>
+        <v>-0.009999999999999998</v>
       </c>
       <c r="D148" t="n">
-        <v>41.24915492957748</v>
+        <v>0.7047945205479452</v>
       </c>
       <c r="E148" t="n">
-        <v>41.24915492957748</v>
+        <v>0.7047945205479452</v>
       </c>
     </row>
     <row r="149">
@@ -2959,16 +2959,16 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>-0.1635211267605634</v>
+        <v>-0.01047945205479452</v>
       </c>
       <c r="C149" t="n">
-        <v>-0.008661971830985915</v>
+        <v>-0.0092</v>
       </c>
       <c r="D149" t="n">
-        <v>41.24915492957748</v>
+        <v>1.103424657534246</v>
       </c>
       <c r="E149" t="n">
-        <v>41.24915492957748</v>
+        <v>1.103424657534246</v>
       </c>
     </row>
     <row r="150">
@@ -2976,16 +2976,16 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>-0.1635211267605634</v>
+        <v>-0.009246575342465754</v>
       </c>
       <c r="C150" t="n">
-        <v>-0.008661971830985915</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="D150" t="n">
-        <v>41.24915492957748</v>
+        <v>-0.4623287671232867</v>
       </c>
       <c r="E150" t="n">
-        <v>41.24915492957748</v>
+        <v>-0.4623287671232867</v>
       </c>
     </row>
     <row r="151">
@@ -2993,16 +2993,16 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0.09422535211267605</v>
+        <v>-0.008835616438356163</v>
       </c>
       <c r="C151" t="n">
-        <v>-0.05471830985915493</v>
+        <v>-0.007599999999999999</v>
       </c>
       <c r="D151" t="n">
-        <v>-277.0964788732394</v>
+        <v>0.2486301369862999</v>
       </c>
       <c r="E151" t="n">
-        <v>-277.0964788732394</v>
+        <v>0.2486301369862999</v>
       </c>
     </row>
     <row r="152">
@@ -3010,16 +3010,16 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0.05492957746478873</v>
+        <v>-0.008013698630136986</v>
       </c>
       <c r="C152" t="n">
-        <v>0.02091549295774648</v>
+        <v>-0.0068</v>
       </c>
       <c r="D152" t="n">
-        <v>36.35577464788732</v>
+        <v>-0.1787671232876707</v>
       </c>
       <c r="E152" t="n">
-        <v>36.35577464788732</v>
+        <v>-0.1787671232876707</v>
       </c>
     </row>
     <row r="153">
@@ -3027,16 +3027,16 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>0.03380281690140845</v>
+        <v>-0.007602739726027397</v>
       </c>
       <c r="C153" t="n">
-        <v>0.06105633802816901</v>
+        <v>-0.005599999999999999</v>
       </c>
       <c r="D153" t="n">
-        <v>19.1830985915493</v>
+        <v>0.1623287671232879</v>
       </c>
       <c r="E153" t="n">
-        <v>19.1830985915493</v>
+        <v>0.1623287671232879</v>
       </c>
     </row>
     <row r="154">
@@ -3044,16 +3044,16 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>0.03718309859154929</v>
+        <v>-0.005958904109589041</v>
       </c>
       <c r="C154" t="n">
-        <v>0.05387323943661972</v>
+        <v>-0.005999999999999999</v>
       </c>
       <c r="D154" t="n">
-        <v>-6.689577464788733</v>
+        <v>-1.062328767123287</v>
       </c>
       <c r="E154" t="n">
-        <v>-6.689577464788733</v>
+        <v>-1.062328767123287</v>
       </c>
     </row>
     <row r="155">
@@ -3061,16 +3061,16 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>0.1305633802816901</v>
+        <v>-0.003904109589041096</v>
       </c>
       <c r="C155" t="n">
-        <v>0.1409154929577465</v>
+        <v>-0.005999999999999999</v>
       </c>
       <c r="D155" t="n">
-        <v>-94.47084507042251</v>
+        <v>-1.576027397260274</v>
       </c>
       <c r="E155" t="n">
-        <v>-94.47084507042251</v>
+        <v>-1.576027397260274</v>
       </c>
     </row>
     <row r="156">
@@ -3078,16 +3078,16 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>0.1263380281690141</v>
+        <v>-0.001849315068493151</v>
       </c>
       <c r="C156" t="n">
-        <v>0.1409154929577465</v>
+        <v>-0.005999999999999999</v>
       </c>
       <c r="D156" t="n">
-        <v>-83.96577464788732</v>
+        <v>-1.71986301369863</v>
       </c>
       <c r="E156" t="n">
-        <v>-83.96577464788732</v>
+        <v>-1.71986301369863</v>
       </c>
     </row>
     <row r="157">
@@ -3095,16 +3095,16 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>0.05746478873239436</v>
+        <v>-0.001027397260273973</v>
       </c>
       <c r="C157" t="n">
-        <v>0.01457746478873239</v>
+        <v>-0.006399999999999999</v>
       </c>
       <c r="D157" t="n">
-        <v>67.01915492957747</v>
+        <v>-0.6678082191780823</v>
       </c>
       <c r="E157" t="n">
-        <v>67.01915492957747</v>
+        <v>-0.6678082191780823</v>
       </c>
     </row>
     <row r="158">
@@ -3112,16 +3112,16 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>0.1301408450704225</v>
+        <v>0.0006164383561643835</v>
       </c>
       <c r="C158" t="n">
-        <v>0.1417605633802817</v>
+        <v>-0.005999999999999999</v>
       </c>
       <c r="D158" t="n">
-        <v>-79.87774647887323</v>
+        <v>-1.522602739726027</v>
       </c>
       <c r="E158" t="n">
-        <v>-79.87774647887323</v>
+        <v>-1.522602739726027</v>
       </c>
     </row>
     <row r="159">
@@ -3129,16 +3129,16 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>0.1297183098591549</v>
+        <v>0.002260273972602739</v>
       </c>
       <c r="C159" t="n">
-        <v>0.1417605633802817</v>
+        <v>-0.006399999999999999</v>
       </c>
       <c r="D159" t="n">
-        <v>-64.40239436619717</v>
+        <v>-1.637671232876712</v>
       </c>
       <c r="E159" t="n">
-        <v>-64.40239436619717</v>
+        <v>-1.637671232876712</v>
       </c>
     </row>
     <row r="160">
@@ -3146,16 +3146,16 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>0.1288732394366197</v>
+        <v>0.003493150684931506</v>
       </c>
       <c r="C160" t="n">
-        <v>0.1417605633802817</v>
+        <v>-0.0072</v>
       </c>
       <c r="D160" t="n">
-        <v>-44.03873239436619</v>
+        <v>-1.354109589041096</v>
       </c>
       <c r="E160" t="n">
-        <v>-44.03873239436619</v>
+        <v>-1.354109589041096</v>
       </c>
     </row>
     <row r="161">
@@ -3163,16 +3163,16 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>0.1309859154929577</v>
+        <v>0.003082191780821918</v>
       </c>
       <c r="C161" t="n">
-        <v>0.1421830985915493</v>
+        <v>-0.0068</v>
       </c>
       <c r="D161" t="n">
-        <v>-44.65943661971831</v>
+        <v>0.1541095890410956</v>
       </c>
       <c r="E161" t="n">
-        <v>-44.65943661971831</v>
+        <v>0.1541095890410956</v>
       </c>
     </row>
     <row r="162">
@@ -3180,16 +3180,16 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>-0.1195774647887324</v>
+        <v>0.004315068493150684</v>
       </c>
       <c r="C162" t="n">
-        <v>-0.1413380281690141</v>
+        <v>-0.008</v>
       </c>
       <c r="D162" t="n">
-        <v>271.7522535211268</v>
+        <v>-1.411643835616438</v>
       </c>
       <c r="E162" t="n">
-        <v>271.7522535211268</v>
+        <v>-1.411643835616438</v>
       </c>
     </row>
     <row r="163">
@@ -3197,16 +3197,16 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>-0.122112676056338</v>
+        <v>0.003082191780821918</v>
       </c>
       <c r="C163" t="n">
-        <v>-0.1388028169014084</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="D163" t="n">
-        <v>13.02633802816902</v>
+        <v>0.8938356164383557</v>
       </c>
       <c r="E163" t="n">
-        <v>13.02633802816902</v>
+        <v>0.8938356164383557</v>
       </c>
     </row>
     <row r="164">
@@ -3214,16 +3214,16 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>-0.1216901408450704</v>
+        <v>0.003493150684931506</v>
       </c>
       <c r="C164" t="n">
-        <v>-0.135</v>
+        <v>-0.0092</v>
       </c>
       <c r="D164" t="n">
-        <v>39.01690140845071</v>
+        <v>-0.6143835616438353</v>
       </c>
       <c r="E164" t="n">
-        <v>39.01690140845071</v>
+        <v>-0.6143835616438353</v>
       </c>
     </row>
     <row r="165">
@@ -3231,16 +3231,16 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>-0.1212676056338028</v>
+        <v>0.002671232876712329</v>
       </c>
       <c r="C165" t="n">
-        <v>-0.135</v>
+        <v>-0.0092</v>
       </c>
       <c r="D165" t="n">
-        <v>39.86323943661971</v>
+        <v>0.5527397260273972</v>
       </c>
       <c r="E165" t="n">
-        <v>39.86323943661971</v>
+        <v>0.5527397260273972</v>
       </c>
     </row>
     <row r="166">
@@ -3248,16 +3248,16 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>-0.1246478873239436</v>
+        <v>0.001849315068493151</v>
       </c>
       <c r="C166" t="n">
-        <v>-0.1345774647887324</v>
+        <v>-0.009999999999999998</v>
       </c>
       <c r="D166" t="n">
-        <v>14.12408450704225</v>
+        <v>0.6102739726027395</v>
       </c>
       <c r="E166" t="n">
-        <v>14.12408450704225</v>
+        <v>0.6102739726027395</v>
       </c>
     </row>
     <row r="167">
@@ -3265,16 +3265,16 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>-0.1246478873239436</v>
+        <v>0.0006164383561643835</v>
       </c>
       <c r="C167" t="n">
-        <v>-0.1345774647887324</v>
+        <v>-0.0104</v>
       </c>
       <c r="D167" t="n">
-        <v>14.12408450704225</v>
+        <v>1.066438356164384</v>
       </c>
       <c r="E167" t="n">
-        <v>14.12408450704225</v>
+        <v>1.066438356164384</v>
       </c>
     </row>
     <row r="168">
@@ -3282,16 +3282,16 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>-0.1246478873239436</v>
+        <v>-0.0002054794520547945</v>
       </c>
       <c r="C168" t="n">
-        <v>-0.1345774647887324</v>
+        <v>-0.0116</v>
       </c>
       <c r="D168" t="n">
-        <v>14.12408450704225</v>
+        <v>0.7541095890410958</v>
       </c>
       <c r="E168" t="n">
-        <v>14.12408450704225</v>
+        <v>0.7541095890410958</v>
       </c>
     </row>
     <row r="169">
@@ -3299,16 +3299,16 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>-0.1246478873239436</v>
+        <v>-0.002260273972602739</v>
       </c>
       <c r="C169" t="n">
-        <v>-0.1345774647887324</v>
+        <v>-0.0116</v>
       </c>
       <c r="D169" t="n">
-        <v>14.12408450704225</v>
+        <v>2.007534246575342</v>
       </c>
       <c r="E169" t="n">
-        <v>14.12408450704225</v>
+        <v>2.007534246575342</v>
       </c>
     </row>
     <row r="170">
@@ -3316,16 +3316,16 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>-0.1246478873239436</v>
+        <v>-0.003082191780821918</v>
       </c>
       <c r="C170" t="n">
-        <v>-0.1345774647887324</v>
+        <v>-0.012</v>
       </c>
       <c r="D170" t="n">
-        <v>14.12408450704225</v>
+        <v>0.9554794520547948</v>
       </c>
       <c r="E170" t="n">
-        <v>14.12408450704225</v>
+        <v>0.9554794520547948</v>
       </c>
     </row>
     <row r="171">
@@ -3333,16 +3333,16 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>-0.1246478873239436</v>
+        <v>-0.004726027397260274</v>
       </c>
       <c r="C171" t="n">
-        <v>-0.1345774647887324</v>
+        <v>-0.0116</v>
       </c>
       <c r="D171" t="n">
-        <v>14.12408450704225</v>
+        <v>1.81027397260274</v>
       </c>
       <c r="E171" t="n">
-        <v>14.12408450704225</v>
+        <v>1.81027397260274</v>
       </c>
     </row>
     <row r="172">
@@ -3350,16 +3350,16 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>0.1136619718309859</v>
+        <v>-0.004315068493150684</v>
       </c>
       <c r="C172" t="n">
-        <v>0.1442957746478873</v>
+        <v>-0.0124</v>
       </c>
       <c r="D172" t="n">
-        <v>-258.4567605633803</v>
+        <v>-0.06780821917808277</v>
       </c>
       <c r="E172" t="n">
-        <v>-258.4567605633803</v>
+        <v>-0.06780821917808277</v>
       </c>
     </row>
     <row r="173">
@@ -3367,16 +3367,16 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.005547945205479451</v>
       </c>
       <c r="C173" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.0112</v>
       </c>
       <c r="D173" t="n">
-        <v>29.45619718309858</v>
+        <v>1.497945205479452</v>
       </c>
       <c r="E173" t="n">
-        <v>29.45619718309858</v>
+        <v>1.497945205479452</v>
       </c>
     </row>
     <row r="174">
@@ -3384,16 +3384,16 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.005547945205479451</v>
       </c>
       <c r="C174" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.0124</v>
       </c>
       <c r="D174" t="n">
-        <v>29.45619718309858</v>
+        <v>0.3883561643835616</v>
       </c>
       <c r="E174" t="n">
-        <v>29.45619718309858</v>
+        <v>0.3883561643835616</v>
       </c>
     </row>
     <row r="175">
@@ -3401,16 +3401,16 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.005958904109589041</v>
       </c>
       <c r="C175" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.0116</v>
       </c>
       <c r="D175" t="n">
-        <v>29.45619718309858</v>
+        <v>0.7869863013698635</v>
       </c>
       <c r="E175" t="n">
-        <v>29.45619718309858</v>
+        <v>0.7869863013698635</v>
       </c>
     </row>
     <row r="176">
@@ -3418,16 +3418,16 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.005958904109589041</v>
       </c>
       <c r="C176" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.0116</v>
       </c>
       <c r="D176" t="n">
-        <v>29.45619718309858</v>
+        <v>0.4171232876712329</v>
       </c>
       <c r="E176" t="n">
-        <v>29.45619718309858</v>
+        <v>0.4171232876712329</v>
       </c>
     </row>
     <row r="177">
@@ -3435,16 +3435,16 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.00636986301369863</v>
       </c>
       <c r="C177" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.0108</v>
       </c>
       <c r="D177" t="n">
-        <v>29.45619718309858</v>
+        <v>0.815753424657534</v>
       </c>
       <c r="E177" t="n">
-        <v>29.45619718309858</v>
+        <v>0.815753424657534</v>
       </c>
     </row>
     <row r="178">
@@ -3452,16 +3452,16 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.00636986301369863</v>
       </c>
       <c r="C178" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.0104</v>
       </c>
       <c r="D178" t="n">
-        <v>29.45619718309858</v>
+        <v>0.4458904109589041</v>
       </c>
       <c r="E178" t="n">
-        <v>29.45619718309858</v>
+        <v>0.4458904109589041</v>
       </c>
     </row>
     <row r="179">
@@ -3469,16 +3469,16 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.005136986301369863</v>
       </c>
       <c r="C179" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.0108</v>
       </c>
       <c r="D179" t="n">
-        <v>29.45619718309858</v>
+        <v>-0.75</v>
       </c>
       <c r="E179" t="n">
-        <v>29.45619718309858</v>
+        <v>-0.75</v>
       </c>
     </row>
     <row r="180">
@@ -3486,16 +3486,16 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.004726027397260274</v>
       </c>
       <c r="C180" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.009999999999999998</v>
       </c>
       <c r="D180" t="n">
-        <v>29.45619718309858</v>
+        <v>-0.03904109589041072</v>
       </c>
       <c r="E180" t="n">
-        <v>29.45619718309858</v>
+        <v>-0.03904109589041072</v>
       </c>
     </row>
     <row r="181">
@@ -3503,16 +3503,16 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.003904109589041096</v>
       </c>
       <c r="C181" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.0104</v>
       </c>
       <c r="D181" t="n">
-        <v>29.45619718309858</v>
+        <v>-0.4664383561643839</v>
       </c>
       <c r="E181" t="n">
-        <v>29.45619718309858</v>
+        <v>-0.4664383561643839</v>
       </c>
     </row>
     <row r="182">
@@ -3520,16 +3520,16 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.003904109589041096</v>
       </c>
       <c r="C182" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.009599999999999999</v>
       </c>
       <c r="D182" t="n">
-        <v>29.45619718309858</v>
+        <v>0.2732876712328767</v>
       </c>
       <c r="E182" t="n">
-        <v>29.45619718309858</v>
+        <v>0.2732876712328767</v>
       </c>
     </row>
     <row r="183">
@@ -3537,16 +3537,16 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.004315068493150684</v>
       </c>
       <c r="C183" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="D183" t="n">
-        <v>29.45619718309858</v>
+        <v>0.6719178082191778</v>
       </c>
       <c r="E183" t="n">
-        <v>29.45619718309858</v>
+        <v>0.6719178082191778</v>
       </c>
     </row>
     <row r="184">
@@ -3554,16 +3554,16 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>0.07901408450704225</v>
+        <v>-0.003082191780821918</v>
       </c>
       <c r="C184" t="n">
-        <v>0.1438732394366197</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="D184" t="n">
-        <v>29.45619718309858</v>
+        <v>-0.8938356164383557</v>
       </c>
       <c r="E184" t="n">
-        <v>29.45619718309858</v>
+        <v>-0.8938356164383557</v>
       </c>
     </row>
     <row r="185">
@@ -3571,16 +3571,16 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>0.1035211267605634</v>
+        <v>-0.002671232876712329</v>
       </c>
       <c r="C185" t="n">
-        <v>-0.07373239436619718</v>
+        <v>-0.008</v>
       </c>
       <c r="D185" t="n">
-        <v>-34.38464788732393</v>
+        <v>-0.1828767123287673</v>
       </c>
       <c r="E185" t="n">
-        <v>-34.38464788732393</v>
+        <v>-0.1828767123287673</v>
       </c>
     </row>
     <row r="186">
@@ -3588,16 +3588,16 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>0.1005633802816901</v>
+        <v>-0.002260273972602739</v>
       </c>
       <c r="C186" t="n">
-        <v>-0.0682394366197183</v>
+        <v>-0.007599999999999999</v>
       </c>
       <c r="D186" t="n">
-        <v>-5.460000000000011</v>
+        <v>-0.2116438356164385</v>
       </c>
       <c r="E186" t="n">
-        <v>-5.460000000000011</v>
+        <v>-0.2116438356164385</v>
       </c>
     </row>
     <row r="187">
@@ -3605,16 +3605,16 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>0.09464788732394365</v>
+        <v>-0.0006164383561643835</v>
       </c>
       <c r="C187" t="n">
-        <v>-0.05683098591549295</v>
+        <v>-0.007599999999999999</v>
       </c>
       <c r="D187" t="n">
-        <v>-1.869295774647877</v>
+        <v>-1.436301369863013</v>
       </c>
       <c r="E187" t="n">
-        <v>-1.869295774647877</v>
+        <v>-1.436301369863013</v>
       </c>
     </row>
     <row r="188">
@@ -3622,16 +3622,16 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>0.0908450704225352</v>
+        <v>-0.001027397260273973</v>
       </c>
       <c r="C188" t="n">
-        <v>-0.04964788732394366</v>
+        <v>-0.0068</v>
       </c>
       <c r="D188" t="n">
-        <v>-3.751690140845072</v>
+        <v>0.4417808219178082</v>
       </c>
       <c r="E188" t="n">
-        <v>-3.751690140845072</v>
+        <v>0.4417808219178082</v>
       </c>
     </row>
     <row r="189">
@@ -3639,16 +3639,16 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>0.09845070422535211</v>
+        <v>-0.001027397260273973</v>
       </c>
       <c r="C189" t="n">
-        <v>-0.06401408450704225</v>
+        <v>-0.0068</v>
       </c>
       <c r="D189" t="n">
-        <v>-16.30859154929578</v>
+        <v>0.07191780821917808</v>
       </c>
       <c r="E189" t="n">
-        <v>-16.30859154929578</v>
+        <v>0.07191780821917808</v>
       </c>
     </row>
     <row r="190">
@@ -3656,16 +3656,16 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>0.09845070422535211</v>
+        <v>-0.001027397260273973</v>
       </c>
       <c r="C190" t="n">
-        <v>-0.06401408450704225</v>
+        <v>-0.0068</v>
       </c>
       <c r="D190" t="n">
-        <v>-16.30859154929578</v>
+        <v>0.07191780821917808</v>
       </c>
       <c r="E190" t="n">
-        <v>-16.30859154929578</v>
+        <v>0.07191780821917808</v>
       </c>
     </row>
     <row r="191">
@@ -3673,16 +3673,16 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>0.09845070422535211</v>
+        <v>-0.0006164383561643835</v>
       </c>
       <c r="C191" t="n">
-        <v>-0.06401408450704225</v>
+        <v>-0.008</v>
       </c>
       <c r="D191" t="n">
-        <v>-16.30859154929578</v>
+        <v>-0.3267123287671232</v>
       </c>
       <c r="E191" t="n">
-        <v>-16.30859154929578</v>
+        <v>-0.3267123287671232</v>
       </c>
     </row>
     <row r="192">
@@ -3690,16 +3690,16 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>0.09845070422535211</v>
+        <v>-0.001438356164383561</v>
       </c>
       <c r="C192" t="n">
-        <v>-0.06401408450704225</v>
+        <v>-0.007599999999999999</v>
       </c>
       <c r="D192" t="n">
-        <v>-16.30859154929578</v>
+        <v>0.8404109589041094</v>
       </c>
       <c r="E192" t="n">
-        <v>-16.30859154929578</v>
+        <v>0.8404109589041094</v>
       </c>
     </row>
     <row r="193">
@@ -3707,16 +3707,16 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>0.09845070422535211</v>
+        <v>-0.001849315068493151</v>
       </c>
       <c r="C193" t="n">
-        <v>-0.06401408450704225</v>
+        <v>-0.007599999999999999</v>
       </c>
       <c r="D193" t="n">
-        <v>-16.30859154929578</v>
+        <v>0.4993150684931508</v>
       </c>
       <c r="E193" t="n">
-        <v>-16.30859154929578</v>
+        <v>0.4993150684931508</v>
       </c>
     </row>
     <row r="194">
@@ -3724,16 +3724,16 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>0.09845070422535211</v>
+        <v>-0.002260273972602739</v>
       </c>
       <c r="C194" t="n">
-        <v>-0.06401408450704225</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="D194" t="n">
-        <v>-16.30859154929578</v>
+        <v>0.5280821917808216</v>
       </c>
       <c r="E194" t="n">
-        <v>-16.30859154929578</v>
+        <v>0.5280821917808216</v>
       </c>
     </row>
     <row r="195">
@@ -3741,16 +3741,16 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>0.09845070422535211</v>
+        <v>-0.003493150684931506</v>
       </c>
       <c r="C195" t="n">
-        <v>-0.06401408450704225</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="D195" t="n">
-        <v>-16.30859154929578</v>
+        <v>1.354109589041096</v>
       </c>
       <c r="E195" t="n">
-        <v>-16.30859154929578</v>
+        <v>1.354109589041096</v>
       </c>
     </row>
     <row r="196">
@@ -3758,16 +3758,16 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>0.09845070422535211</v>
+        <v>-0.004315068493150684</v>
       </c>
       <c r="C196" t="n">
-        <v>-0.06401408450704225</v>
+        <v>-0.0092</v>
       </c>
       <c r="D196" t="n">
-        <v>-16.30859154929578</v>
+        <v>1.041780821917808</v>
       </c>
       <c r="E196" t="n">
-        <v>-16.30859154929578</v>
+        <v>1.041780821917808</v>
       </c>
     </row>
     <row r="197">
@@ -3775,16 +3775,16 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>-0.1432394366197183</v>
+        <v>-0.003904109589041096</v>
       </c>
       <c r="C197" t="n">
-        <v>0.1472535211267605</v>
+        <v>-0.0104</v>
       </c>
       <c r="D197" t="n">
-        <v>264.4998591549295</v>
+        <v>-0.09657534246575322</v>
       </c>
       <c r="E197" t="n">
-        <v>264.4998591549295</v>
+        <v>-0.09657534246575322</v>
       </c>
     </row>
     <row r="198">
@@ -3792,16 +3792,16 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>-0.1191549295774648</v>
+        <v>-0.004726027397260274</v>
       </c>
       <c r="C198" t="n">
-        <v>-0.1413380281690141</v>
+        <v>-0.009999999999999998</v>
       </c>
       <c r="D198" t="n">
-        <v>-15.01605633802818</v>
+        <v>1.07054794520548</v>
       </c>
       <c r="E198" t="n">
-        <v>-15.01605633802818</v>
+        <v>1.07054794520548</v>
       </c>
     </row>
     <row r="199">
@@ -3809,16 +3809,16 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>-0.1330985915492958</v>
+        <v>-0.004315068493150684</v>
       </c>
       <c r="C199" t="n">
-        <v>0.1476760563380282</v>
+        <v>-0.0108</v>
       </c>
       <c r="D199" t="n">
-        <v>235.4057746478873</v>
+        <v>-0.06780821917808277</v>
       </c>
       <c r="E199" t="n">
-        <v>235.4057746478873</v>
+        <v>-0.06780821917808277</v>
       </c>
     </row>
     <row r="200">
@@ -3826,16 +3826,16 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>-0.1398591549295775</v>
+        <v>-0.004315068493150684</v>
       </c>
       <c r="C200" t="n">
-        <v>0.1476760563380282</v>
+        <v>-0.0108</v>
       </c>
       <c r="D200" t="n">
-        <v>200.6902816901408</v>
+        <v>0.3020547945205479</v>
       </c>
       <c r="E200" t="n">
-        <v>200.6902816901408</v>
+        <v>0.3020547945205479</v>
       </c>
     </row>
     <row r="201">
@@ -3843,16 +3843,16 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>-0.1419718309859155</v>
+        <v>-0.004315068493150684</v>
       </c>
       <c r="C201" t="n">
-        <v>0.1472535211267605</v>
+        <v>-0.0108</v>
       </c>
       <c r="D201" t="n">
-        <v>196.8997183098591</v>
+        <v>0.3020547945205479</v>
       </c>
       <c r="E201" t="n">
-        <v>196.8997183098591</v>
+        <v>0.3020547945205479</v>
       </c>
     </row>
     <row r="202">
@@ -3860,16 +3860,16 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>-0.1377464788732394</v>
+        <v>-0.004315068493150684</v>
       </c>
       <c r="C202" t="n">
-        <v>0.1472535211267605</v>
+        <v>-0.0108</v>
       </c>
       <c r="D202" t="n">
-        <v>193.8938028169014</v>
+        <v>0.3020547945205479</v>
       </c>
       <c r="E202" t="n">
-        <v>193.8938028169014</v>
+        <v>0.3020547945205479</v>
       </c>
     </row>
     <row r="203">
@@ -3877,16 +3877,16 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
-        <v>0.04014084507042253</v>
+        <v>-0.004726027397260274</v>
       </c>
       <c r="C203" t="n">
-        <v>0.04880281690140845</v>
+        <v>-0.009999999999999998</v>
       </c>
       <c r="D203" t="n">
-        <v>-189.126338028169</v>
+        <v>0.7006849315068499</v>
       </c>
       <c r="E203" t="n">
-        <v>-189.126338028169</v>
+        <v>0.7006849315068499</v>
       </c>
     </row>
     <row r="204">
@@ -3894,16 +3894,16 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
-        <v>0.04605633802816901</v>
+        <v>-0.003904109589041096</v>
       </c>
       <c r="C204" t="n">
-        <v>0.0378169014084507</v>
+        <v>-0.0104</v>
       </c>
       <c r="D204" t="n">
-        <v>-10.09056338028169</v>
+        <v>-0.4664383561643839</v>
       </c>
       <c r="E204" t="n">
-        <v>-10.09056338028169</v>
+        <v>-0.4664383561643839</v>
       </c>
     </row>
     <row r="205">
@@ -3911,16 +3911,16 @@
         <v>203</v>
       </c>
       <c r="B205" t="n">
-        <v>0.05577464788732394</v>
+        <v>-0.002671232876712329</v>
       </c>
       <c r="C205" t="n">
-        <v>0.01964788732394366</v>
+        <v>-0.009999999999999998</v>
       </c>
       <c r="D205" t="n">
-        <v>-14.88676056338028</v>
+        <v>-0.9226027397260275</v>
       </c>
       <c r="E205" t="n">
-        <v>-14.88676056338028</v>
+        <v>-0.9226027397260275</v>
       </c>
     </row>
     <row r="206">
@@ -3928,16 +3928,16 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>0.06633802816901407</v>
+        <v>-0.003082191780821918</v>
       </c>
       <c r="C206" t="n">
-        <v>-0.0006338028169014084</v>
+        <v>-0.0092</v>
       </c>
       <c r="D206" t="n">
-        <v>-16.66690140845069</v>
+        <v>0.5856164383561645</v>
       </c>
       <c r="E206" t="n">
-        <v>-16.66690140845069</v>
+        <v>0.5856164383561645</v>
       </c>
     </row>
     <row r="207">
@@ -3945,16 +3945,16 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>0.08408450704225351</v>
+        <v>-0.002260273972602739</v>
       </c>
       <c r="C207" t="n">
-        <v>-0.03528169014084507</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="D207" t="n">
-        <v>-25.67450704225352</v>
+        <v>-0.5815068493150688</v>
       </c>
       <c r="E207" t="n">
-        <v>-25.67450704225352</v>
+        <v>-0.5815068493150688</v>
       </c>
     </row>
     <row r="208">
@@ -3962,16 +3962,16 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>0.08408450704225351</v>
+        <v>-0.002260273972602739</v>
       </c>
       <c r="C208" t="n">
-        <v>-0.03528169014084507</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="D208" t="n">
-        <v>-25.67450704225352</v>
+        <v>0.1582191780821918</v>
       </c>
       <c r="E208" t="n">
-        <v>-25.67450704225352</v>
+        <v>0.1582191780821918</v>
       </c>
     </row>
     <row r="209">
@@ -3979,16 +3979,16 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>0.1309859154929577</v>
+        <v>-0.001438356164383561</v>
       </c>
       <c r="C209" t="n">
-        <v>0.1434507042253521</v>
+        <v>-0.008</v>
       </c>
       <c r="D209" t="n">
-        <v>-60.09887323943662</v>
+        <v>-0.6390410958904108</v>
       </c>
       <c r="E209" t="n">
-        <v>-60.09887323943662</v>
+        <v>-0.6390410958904108</v>
       </c>
     </row>
     <row r="210">
@@ -3996,16 +3996,16 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>0.1238028169014084</v>
+        <v>-0.0006164383561643835</v>
       </c>
       <c r="C210" t="n">
-        <v>0.1400704225352113</v>
+        <v>-0.0072</v>
       </c>
       <c r="D210" t="n">
-        <v>-297.2556338028169</v>
+        <v>-0.6965753424657533</v>
       </c>
       <c r="E210" t="n">
-        <v>-297.2556338028169</v>
+        <v>-0.6965753424657533</v>
       </c>
     </row>
     <row r="211">
@@ -4013,101 +4013,16 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>0.1191549295774648</v>
+        <v>-0.0006164383561643835</v>
       </c>
       <c r="C211" t="n">
-        <v>0.132887323943662</v>
+        <v>-0.005999999999999999</v>
       </c>
       <c r="D211" t="n">
-        <v>-298.6250704225351</v>
+        <v>0.04315068493150685</v>
       </c>
       <c r="E211" t="n">
-        <v>-298.6250704225351</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" s="1" t="n">
-        <v>210</v>
-      </c>
-      <c r="B212" t="n">
-        <v>0.1229577464788732</v>
-      </c>
-      <c r="C212" t="n">
-        <v>0.1366901408450704</v>
-      </c>
-      <c r="D212" t="n">
-        <v>-302.9184507042252</v>
-      </c>
-      <c r="E212" t="n">
-        <v>-302.9184507042252</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" s="1" t="n">
-        <v>211</v>
-      </c>
-      <c r="B213" t="n">
-        <v>0.1259154929577465</v>
-      </c>
-      <c r="C213" t="n">
-        <v>0.1434507042253521</v>
-      </c>
-      <c r="D213" t="n">
-        <v>-306.2577464788732</v>
-      </c>
-      <c r="E213" t="n">
-        <v>-306.2577464788732</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" s="1" t="n">
-        <v>212</v>
-      </c>
-      <c r="B214" t="n">
-        <v>-0.1588732394366197</v>
-      </c>
-      <c r="C214" t="n">
-        <v>0.146830985915493</v>
-      </c>
-      <c r="D214" t="n">
-        <v>58.94028169014084</v>
-      </c>
-      <c r="E214" t="n">
-        <v>58.94028169014084</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" s="1" t="n">
-        <v>213</v>
-      </c>
-      <c r="B215" t="n">
-        <v>-0.1597183098591549</v>
-      </c>
-      <c r="C215" t="n">
-        <v>0.1455633802816901</v>
-      </c>
-      <c r="D215" t="n">
-        <v>50.18957746478873</v>
-      </c>
-      <c r="E215" t="n">
-        <v>50.18957746478873</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" s="1" t="n">
-        <v>214</v>
-      </c>
-      <c r="B216" t="n">
-        <v>-0.1554929577464789</v>
-      </c>
-      <c r="C216" t="n">
-        <v>0.1459859154929577</v>
-      </c>
-      <c r="D216" t="n">
-        <v>43.21352112676055</v>
-      </c>
-      <c r="E216" t="n">
-        <v>43.21352112676055</v>
+        <v>0.04315068493150685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>